<commit_message>
luxiongbo add source table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404"/>
   </bookViews>
   <sheets>
     <sheet name="总览" sheetId="1" r:id="rId1"/>
@@ -997,6 +997,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1006,23 +1018,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1345,7 +1345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20:G26"/>
     </sheetView>
   </sheetViews>
@@ -1366,20 +1366,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
       <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="25" t="s">
         <v>139</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1416,7 +1416,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1425,7 +1425,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="23" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1434,8 +1434,8 @@
       <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="21" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="24" t="s">
         <v>135</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1447,22 +1447,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="21"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="4" t="s">
         <v>133</v>
       </c>
@@ -1472,22 +1472,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="19"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="24"/>
       <c r="J5" s="4" t="s">
         <v>134</v>
       </c>
@@ -1497,39 +1497,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="25"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="19"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="5" t="s">
         <v>142</v>
       </c>
@@ -1542,15 +1542,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="21" t="s">
+      <c r="H8" s="25"/>
+      <c r="I8" s="24" t="s">
         <v>144</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1562,7 +1562,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1578,8 +1578,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="21"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="4" t="s">
         <v>140</v>
       </c>
@@ -1589,7 +1589,7 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1605,8 +1605,8 @@
       <c r="G10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="21"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="4" t="s">
         <v>141</v>
       </c>
@@ -1616,7 +1616,7 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
@@ -1630,11 +1630,11 @@
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="25"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
@@ -1648,7 +1648,7 @@
       <c r="G12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="5" t="s">
         <v>145</v>
       </c>
@@ -1661,7 +1661,7 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
@@ -1675,8 +1675,8 @@
       <c r="G13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="21" t="s">
+      <c r="H13" s="25"/>
+      <c r="I13" s="24" t="s">
         <v>148</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1688,7 +1688,7 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2" t="s">
         <v>48</v>
       </c>
@@ -1702,8 +1702,8 @@
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="21"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="4" t="s">
         <v>146</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
@@ -1727,8 +1727,8 @@
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="21"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="4" t="s">
         <v>147</v>
       </c>
@@ -1745,7 +1745,7 @@
       <c r="G16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="25"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1765,16 +1765,16 @@
       <c r="G17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23" t="s">
+      <c r="H17" s="25"/>
+      <c r="I17" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="23" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1790,27 +1790,27 @@
       <c r="G18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="25"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23" t="s">
+      <c r="H19" s="25"/>
+      <c r="I19" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1826,7 +1826,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="22"/>
+      <c r="H20" s="25"/>
       <c r="I20" s="2" t="s">
         <v>170</v>
       </c>
@@ -1839,7 +1839,7 @@
       <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
@@ -1855,7 +1855,7 @@
       <c r="G21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="25"/>
       <c r="I21" s="20" t="s">
         <v>169</v>
       </c>
@@ -1868,7 +1868,7 @@
       <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="2" t="s">
         <v>92</v>
       </c>
@@ -1882,7 +1882,7 @@
       <c r="G22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="22"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="20"/>
       <c r="J22" s="1" t="s">
         <v>166</v>
@@ -1893,7 +1893,7 @@
       <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
@@ -1907,7 +1907,7 @@
       <c r="G23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="22"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="20"/>
       <c r="J23" s="1" t="s">
         <v>167</v>
@@ -1918,7 +1918,7 @@
       <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
@@ -1932,7 +1932,7 @@
       <c r="G24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H24" s="22"/>
+      <c r="H24" s="25"/>
       <c r="I24" s="20"/>
       <c r="J24" s="1" t="s">
         <v>168</v>
@@ -1950,7 +1950,7 @@
       <c r="G25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="22"/>
+      <c r="H25" s="25"/>
       <c r="I25" s="20"/>
       <c r="J25" s="1" t="s">
         <v>171</v>
@@ -1970,14 +1970,14 @@
       <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="24" t="s">
+      <c r="E26" s="18"/>
+      <c r="F26" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="G26" s="24" t="s">
+      <c r="G26" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="H26" s="22"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="20"/>
       <c r="J26" s="1" t="s">
         <v>172</v>
@@ -1988,7 +1988,7 @@
       <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="23" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2006,7 +2006,7 @@
       <c r="G27" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="20"/>
       <c r="J27" s="1" t="s">
         <v>173</v>
@@ -2017,14 +2017,14 @@
       <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="22" t="s">
         <v>79</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2033,7 +2033,7 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="25"/>
       <c r="I28" s="20"/>
       <c r="J28" s="1" t="s">
         <v>174</v>
@@ -2044,21 +2044,21 @@
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="25"/>
       <c r="I29" s="20"/>
       <c r="J29" s="1" t="s">
         <v>175</v>
@@ -2069,21 +2069,21 @@
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="18"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="22"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="20"/>
       <c r="J30" s="1" t="s">
         <v>176</v>
@@ -2094,21 +2094,21 @@
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="18"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="22"/>
+      <c r="H31" s="25"/>
       <c r="I31" s="20"/>
       <c r="J31" s="1" t="s">
         <v>177</v>
@@ -2119,100 +2119,100 @@
       <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="18"/>
+      <c r="E32" s="22"/>
       <c r="F32" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="22"/>
+      <c r="H32" s="25"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="18"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="21" t="s">
+      <c r="H33" s="25"/>
+      <c r="I33" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="18"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="18"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="8" t="s">
         <v>78</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E36" s="18"/>
+      <c r="E36" s="22"/>
       <c r="F36" s="8" t="s">
         <v>85</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H36" s="22"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2225,21 +2225,21 @@
       <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="18"/>
+      <c r="E37" s="22"/>
       <c r="F37" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="23" t="s">
         <v>130</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2248,35 +2248,35 @@
       <c r="C38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="18"/>
+      <c r="E38" s="22"/>
       <c r="F38" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="2" t="s">
         <v>125</v>
       </c>
@@ -2292,14 +2292,14 @@
       <c r="G40" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H40" s="22"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="2" t="s">
         <v>121</v>
       </c>
@@ -2315,14 +2315,14 @@
       <c r="G41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="2" t="s">
         <v>92</v>
       </c>
@@ -2336,14 +2336,14 @@
       <c r="G42" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H42" s="22"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="2" t="s">
         <v>122</v>
       </c>
@@ -2357,14 +2357,14 @@
       <c r="G43" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="2" t="s">
         <v>123</v>
       </c>
@@ -2376,14 +2376,14 @@
       <c r="G44" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H44" s="22"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="2" t="s">
         <v>126</v>
       </c>
@@ -2397,14 +2397,14 @@
       <c r="G45" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="2" t="s">
         <v>127</v>
       </c>
@@ -2416,10 +2416,10 @@
       <c r="G46" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="21"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -2456,6 +2456,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="I17:K17"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="I21:I31"/>
     <mergeCell ref="A1:L1"/>
@@ -2472,8 +2474,6 @@
     <mergeCell ref="A18:A24"/>
     <mergeCell ref="I33:K46"/>
     <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2485,8 +2485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2509,7 +2509,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2520,7 +2520,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="23"/>
       <c r="B3" s="1" t="s">
         <v>111</v>
       </c>
@@ -2529,7 +2529,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="1" t="s">
         <v>112</v>
       </c>
@@ -2538,7 +2538,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="1" t="s">
         <v>109</v>
       </c>
@@ -2547,7 +2547,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
@@ -2556,7 +2556,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="1" t="s">
         <v>191</v>
       </c>
@@ -2565,7 +2565,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="1" t="s">
         <v>194</v>
       </c>
@@ -2574,7 +2574,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="1" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
lixiongbo add supervisortype table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -1004,6 +1004,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
@@ -1020,9 +1023,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:G26"/>
+      <selection activeCell="I8" sqref="I8:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1366,20 +1366,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
       <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="19" t="s">
         <v>139</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1416,7 +1416,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1425,7 +1425,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="24" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1434,8 +1434,8 @@
       <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="19"/>
+      <c r="I3" s="25" t="s">
         <v>135</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1447,22 +1447,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="24"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="25"/>
       <c r="J4" s="4" t="s">
         <v>133</v>
       </c>
@@ -1472,22 +1472,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="24"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="25"/>
       <c r="J5" s="4" t="s">
         <v>134</v>
       </c>
@@ -1497,39 +1497,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="25"/>
+      <c r="H6" s="19"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="25"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="5" t="s">
         <v>142</v>
       </c>
@@ -1542,15 +1542,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="24" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="25" t="s">
         <v>144</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1562,7 +1562,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1578,8 +1578,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="24"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="25"/>
       <c r="J9" s="4" t="s">
         <v>140</v>
       </c>
@@ -1589,14 +1589,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="21" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1605,8 +1605,8 @@
       <c r="G10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="24"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="4" t="s">
         <v>141</v>
       </c>
@@ -1616,39 +1616,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="19"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="25"/>
+      <c r="H12" s="19"/>
       <c r="I12" s="5" t="s">
         <v>145</v>
       </c>
@@ -1661,22 +1661,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="24" t="s">
+      <c r="H13" s="19"/>
+      <c r="I13" s="25" t="s">
         <v>148</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1688,22 +1688,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="24"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="4" t="s">
         <v>146</v>
       </c>
@@ -1713,22 +1713,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="24"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="25"/>
       <c r="J15" s="4" t="s">
         <v>147</v>
       </c>
@@ -1738,14 +1738,14 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="25"/>
+      <c r="H16" s="19"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1758,23 +1758,23 @@
       <c r="C17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="19" t="s">
+      <c r="H17" s="19"/>
+      <c r="I17" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="24" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1783,34 +1783,34 @@
       <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="25"/>
+      <c r="H18" s="19"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="19"/>
+      <c r="I19" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1826,7 +1826,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="25"/>
+      <c r="H20" s="19"/>
       <c r="I20" s="2" t="s">
         <v>170</v>
       </c>
@@ -1839,14 +1839,14 @@
       <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="21" t="s">
         <v>116</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1855,8 +1855,8 @@
       <c r="G21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="20" t="s">
+      <c r="H21" s="19"/>
+      <c r="I21" s="21" t="s">
         <v>169</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1868,22 +1868,22 @@
       <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="21"/>
       <c r="F22" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="20"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="1" t="s">
         <v>166</v>
       </c>
@@ -1893,22 +1893,22 @@
       <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="20"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="1" t="s">
         <v>112</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="20"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="1" t="s">
         <v>167</v>
       </c>
@@ -1918,22 +1918,22 @@
       <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="1" t="s">
         <v>109</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="20"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="1" t="s">
         <v>168</v>
       </c>
@@ -1943,15 +1943,15 @@
       <c r="L24" s="13"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="20"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="20"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="1" t="s">
         <v>171</v>
       </c>
@@ -1977,8 +1977,8 @@
       <c r="G26" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="20"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="1" t="s">
         <v>172</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2006,8 +2006,8 @@
       <c r="G27" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="20"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="1" t="s">
         <v>173</v>
       </c>
@@ -2017,14 +2017,14 @@
       <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="23" t="s">
         <v>79</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2033,8 +2033,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="25"/>
-      <c r="I28" s="20"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="1" t="s">
         <v>174</v>
       </c>
@@ -2044,22 +2044,22 @@
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="22"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="1" t="s">
         <v>175</v>
       </c>
@@ -2069,22 +2069,22 @@
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="22"/>
+      <c r="E30" s="23"/>
       <c r="F30" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="20"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="1" t="s">
         <v>176</v>
       </c>
@@ -2094,22 +2094,22 @@
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="22"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="20"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="1" t="s">
         <v>177</v>
       </c>
@@ -2119,100 +2119,100 @@
       <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="22"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="25"/>
+      <c r="H32" s="19"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="22"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="25"/>
-      <c r="I33" s="24" t="s">
+      <c r="H33" s="19"/>
+      <c r="I33" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="22"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="25"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="22"/>
+      <c r="E35" s="23"/>
       <c r="F35" s="8" t="s">
         <v>78</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E36" s="22"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="8" t="s">
         <v>85</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H36" s="25"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2225,21 +2225,21 @@
       <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="22"/>
+      <c r="E37" s="23"/>
       <c r="F37" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="24" t="s">
         <v>130</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2248,35 +2248,35 @@
       <c r="C38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="22"/>
+      <c r="E38" s="23"/>
       <c r="F38" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="25"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="2" t="s">
         <v>125</v>
       </c>
@@ -2292,21 +2292,21 @@
       <c r="G40" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="21" t="s">
         <v>157</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2315,111 +2315,111 @@
       <c r="G41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="25"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="20"/>
+      <c r="E42" s="21"/>
       <c r="F42" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E43" s="20"/>
+      <c r="E43" s="21"/>
       <c r="F43" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H43" s="25"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="21"/>
       <c r="F44" s="9" t="s">
         <v>155</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H44" s="25"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E45" s="20"/>
+      <c r="E45" s="21"/>
       <c r="F45" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="25"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="20"/>
+      <c r="E46" s="21"/>
       <c r="F46" s="9" t="s">
         <v>156</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="H46" s="25"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -2456,6 +2456,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="I33:K46"/>
+    <mergeCell ref="E41:E46"/>
     <mergeCell ref="H2:H46"/>
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="I19:K19"/>
@@ -2472,8 +2474,6 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="A18:A24"/>
-    <mergeCell ref="I33:K46"/>
-    <mergeCell ref="E41:E46"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2509,7 +2509,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2520,7 +2520,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="1" t="s">
         <v>111</v>
       </c>
@@ -2529,7 +2529,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>112</v>
       </c>
@@ -2538,7 +2538,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>109</v>
       </c>
@@ -2547,7 +2547,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
@@ -2556,7 +2556,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>191</v>
       </c>
@@ -2565,7 +2565,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>194</v>
       </c>
@@ -2574,7 +2574,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="1" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
luxiongbo add laboratory info table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="200">
   <si>
     <t>TEACHER_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -821,6 +821,10 @@
   </si>
   <si>
     <t>期刊会议名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个表只有一行记录，就是显示实验室的信息</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -828,7 +832,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -867,8 +871,17 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -909,8 +922,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -933,8 +951,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -944,8 +977,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1003,15 +1039,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1021,16 +1060,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="差" xfId="1" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="检查单元格" xfId="3" builtinId="23"/>
     <cellStyle name="适中" xfId="2" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1345,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:I10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1366,23 +1409,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
       <c r="M1" s="15"/>
     </row>
-    <row r="2" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>24</v>
       </c>
@@ -1401,7 +1444,7 @@
       <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="21" t="s">
         <v>139</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1415,8 +1458,8 @@
       </c>
       <c r="L2" s="13"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1425,7 +1468,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1434,8 +1477,8 @@
       <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="25" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="27" t="s">
         <v>135</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1446,23 +1489,23 @@
       </c>
       <c r="L3" s="13"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+    <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="25"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="27"/>
       <c r="J4" s="4" t="s">
         <v>133</v>
       </c>
@@ -1471,23 +1514,23 @@
       </c>
       <c r="L4" s="13"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+    <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="25"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="25"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="27"/>
       <c r="J5" s="4" t="s">
         <v>134</v>
       </c>
@@ -1496,40 +1539,40 @@
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+    <row r="6" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="19"/>
+      <c r="H6" s="21"/>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+    <row r="7" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="25"/>
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="19"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="5" t="s">
         <v>142</v>
       </c>
@@ -1541,16 +1584,16 @@
       </c>
       <c r="L7" s="13"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+    <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
       <c r="B8" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="25" t="s">
+      <c r="H8" s="21"/>
+      <c r="I8" s="27" t="s">
         <v>144</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1561,8 +1604,8 @@
       </c>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+    <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="25"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1578,8 +1621,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="25"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="27"/>
       <c r="J9" s="4" t="s">
         <v>140</v>
       </c>
@@ -1588,15 +1631,15 @@
       </c>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
+    <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1605,8 +1648,8 @@
       <c r="G10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="25"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="4" t="s">
         <v>141</v>
       </c>
@@ -1615,40 +1658,40 @@
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+    <row r="11" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="19"/>
+      <c r="H11" s="21"/>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+    <row r="12" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25"/>
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="21"/>
       <c r="I12" s="5" t="s">
         <v>145</v>
       </c>
@@ -1660,23 +1703,23 @@
       </c>
       <c r="L12" s="13"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+    <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25"/>
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="25" t="s">
+      <c r="H13" s="21"/>
+      <c r="I13" s="27" t="s">
         <v>148</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1687,23 +1730,23 @@
       </c>
       <c r="L13" s="13"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+    <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25"/>
       <c r="B14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="25"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="27"/>
       <c r="J14" s="4" t="s">
         <v>146</v>
       </c>
@@ -1712,23 +1755,23 @@
       </c>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+    <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25"/>
       <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="25"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="27"/>
       <c r="J15" s="4" t="s">
         <v>147</v>
       </c>
@@ -1737,18 +1780,18 @@
       </c>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E16" s="21"/>
+    <row r="16" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="20"/>
       <c r="F16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="19"/>
+      <c r="H16" s="21"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>117</v>
       </c>
@@ -1758,23 +1801,23 @@
       <c r="C17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="21"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="20" t="s">
+      <c r="H17" s="21"/>
+      <c r="I17" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1783,34 +1826,34 @@
       <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="21"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="19"/>
+      <c r="H18" s="21"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
       <c r="B19" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="20" t="s">
+      <c r="H19" s="21"/>
+      <c r="I19" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+    <row r="20" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
       <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1826,7 +1869,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="19"/>
+      <c r="H20" s="21"/>
       <c r="I20" s="2" t="s">
         <v>170</v>
       </c>
@@ -1837,16 +1880,19 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="M20" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="27" t="s">
         <v>116</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1855,8 +1901,8 @@
       <c r="G21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="21" t="s">
+      <c r="H21" s="21"/>
+      <c r="I21" s="27" t="s">
         <v>169</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1866,24 +1912,25 @@
         <v>178</v>
       </c>
       <c r="L21" s="13"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="M21" s="28"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
       <c r="B22" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="27"/>
       <c r="F22" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="27"/>
       <c r="J22" s="1" t="s">
         <v>166</v>
       </c>
@@ -1891,24 +1938,25 @@
         <v>179</v>
       </c>
       <c r="L22" s="13"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="M22" s="28"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25"/>
       <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="21"/>
+      <c r="E23" s="27"/>
       <c r="F23" s="1" t="s">
         <v>112</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="27"/>
       <c r="J23" s="1" t="s">
         <v>167</v>
       </c>
@@ -1916,24 +1964,25 @@
         <v>181</v>
       </c>
       <c r="L23" s="13"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="M23" s="28"/>
+    </row>
+    <row r="24" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
       <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="21"/>
+      <c r="E24" s="27"/>
       <c r="F24" s="1" t="s">
         <v>109</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="27"/>
       <c r="J24" s="1" t="s">
         <v>168</v>
       </c>
@@ -1941,17 +1990,18 @@
         <v>180</v>
       </c>
       <c r="L24" s="13"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="21"/>
+      <c r="M24" s="28"/>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="27"/>
       <c r="F25" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="27"/>
       <c r="J25" s="1" t="s">
         <v>171</v>
       </c>
@@ -1959,8 +2009,9 @@
         <v>182</v>
       </c>
       <c r="L25" s="13"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="28"/>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -1977,8 +2028,8 @@
       <c r="G26" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="27"/>
       <c r="J26" s="1" t="s">
         <v>172</v>
       </c>
@@ -1986,9 +2037,10 @@
         <v>183</v>
       </c>
       <c r="L26" s="13"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="M26" s="28"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2006,8 +2058,8 @@
       <c r="G27" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="19"/>
-      <c r="I27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="27"/>
       <c r="J27" s="1" t="s">
         <v>173</v>
       </c>
@@ -2015,16 +2067,17 @@
         <v>184</v>
       </c>
       <c r="L27" s="13"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="M27" s="28"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25"/>
       <c r="B28" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="24" t="s">
         <v>79</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2033,8 +2086,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="27"/>
       <c r="J28" s="1" t="s">
         <v>174</v>
       </c>
@@ -2042,24 +2095,25 @@
         <v>185</v>
       </c>
       <c r="L28" s="13"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="M28" s="28"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25"/>
       <c r="B29" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="23"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="27"/>
       <c r="J29" s="1" t="s">
         <v>175</v>
       </c>
@@ -2067,24 +2121,25 @@
         <v>186</v>
       </c>
       <c r="L29" s="13"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="M29" s="28"/>
+    </row>
+    <row r="30" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="23"/>
+      <c r="E30" s="24"/>
       <c r="F30" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="27"/>
       <c r="J30" s="1" t="s">
         <v>176</v>
       </c>
@@ -2092,24 +2147,25 @@
         <v>187</v>
       </c>
       <c r="L30" s="13"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="M30" s="28"/>
+    </row>
+    <row r="31" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="25"/>
       <c r="B31" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="23"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="27"/>
       <c r="J31" s="1" t="s">
         <v>177</v>
       </c>
@@ -2117,102 +2173,103 @@
         <v>188</v>
       </c>
       <c r="L31" s="13"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="M31" s="28"/>
+    </row>
+    <row r="32" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
       <c r="B32" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="23"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="19"/>
+      <c r="H32" s="21"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="23"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="19"/>
-      <c r="I33" s="25" t="s">
+      <c r="H33" s="21"/>
+      <c r="I33" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="23"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="19"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="23"/>
+      <c r="E35" s="24"/>
       <c r="F35" s="8" t="s">
         <v>78</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E36" s="23"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="8" t="s">
         <v>85</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H36" s="19"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2225,21 +2282,21 @@
       <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="23"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="19"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="25" t="s">
         <v>130</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2248,35 +2305,35 @@
       <c r="C38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="19"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H39" s="19"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="2" t="s">
         <v>125</v>
       </c>
@@ -2292,21 +2349,21 @@
       <c r="G40" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H40" s="19"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="20" t="s">
         <v>157</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2315,111 +2372,111 @@
       <c r="G41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="21"/>
+      <c r="E42" s="20"/>
       <c r="F42" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H42" s="19"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="20"/>
       <c r="F43" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H43" s="19"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="21"/>
+      <c r="E44" s="20"/>
       <c r="F44" s="9" t="s">
         <v>155</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H44" s="19"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E45" s="21"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="19"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="21"/>
+      <c r="E46" s="20"/>
       <c r="F46" s="9" t="s">
         <v>156</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="H46" s="19"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -2455,13 +2512,8 @@
       <c r="H53" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="I33:K46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
+  <mergeCells count="19">
+    <mergeCell ref="M20:M31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
     <mergeCell ref="A27:A35"/>
@@ -2474,6 +2526,12 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="A18:A24"/>
+    <mergeCell ref="I33:K46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2509,7 +2567,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2520,7 +2578,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="1" t="s">
         <v>111</v>
       </c>
@@ -2529,7 +2587,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="1" t="s">
         <v>112</v>
       </c>
@@ -2538,7 +2596,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="1" t="s">
         <v>109</v>
       </c>
@@ -2547,7 +2605,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
@@ -2556,7 +2614,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="1" t="s">
         <v>191</v>
       </c>
@@ -2565,7 +2623,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="1" t="s">
         <v>194</v>
       </c>
@@ -2574,7 +2632,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="1" t="s">
         <v>197</v>
       </c>

</xml_diff>

<commit_message>
luxiongbo add news table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="201">
   <si>
     <t>TEACHER_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -825,6 +825,10 @@
   </si>
   <si>
     <t>这个表只有一行记录，就是显示实验室的信息</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -981,7 +985,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1039,35 +1043,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1386,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1409,20 +1410,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1444,7 +1445,7 @@
       <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="25" t="s">
         <v>139</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1459,7 +1460,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1468,7 +1469,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="21" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1477,8 +1478,8 @@
       <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="27" t="s">
+      <c r="H3" s="25"/>
+      <c r="I3" s="22" t="s">
         <v>135</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1490,22 +1491,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="27"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="22"/>
       <c r="J4" s="4" t="s">
         <v>133</v>
       </c>
@@ -1515,22 +1516,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="27"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="4" t="s">
         <v>134</v>
       </c>
@@ -1540,39 +1541,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="25"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="5" t="s">
         <v>142</v>
       </c>
@@ -1585,15 +1586,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="2" t="s">
         <v>131</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="27" t="s">
+      <c r="H8" s="25"/>
+      <c r="I8" s="22" t="s">
         <v>144</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1605,7 +1606,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1621,8 +1622,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="27"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="4" t="s">
         <v>140</v>
       </c>
@@ -1632,14 +1633,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="23" t="s">
         <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1648,8 +1649,8 @@
       <c r="G10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="27"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="22"/>
       <c r="J10" s="4" t="s">
         <v>141</v>
       </c>
@@ -1659,39 +1660,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="23"/>
       <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="21"/>
+      <c r="H11" s="25"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="21"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="5" t="s">
         <v>145</v>
       </c>
@@ -1704,22 +1705,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="27" t="s">
+      <c r="H13" s="25"/>
+      <c r="I13" s="22" t="s">
         <v>148</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1731,22 +1732,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="27"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="4" t="s">
         <v>146</v>
       </c>
@@ -1756,22 +1757,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="27"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="4" t="s">
         <v>147</v>
       </c>
@@ -1781,17 +1782,17 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="20"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="21"/>
+      <c r="H16" s="25"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>117</v>
       </c>
@@ -1801,23 +1802,23 @@
       <c r="C17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="20"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="22" t="s">
+      <c r="H17" s="25"/>
+      <c r="I17" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1826,34 +1827,34 @@
       <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="21"/>
+      <c r="H18" s="25"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
       <c r="B19" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="22" t="s">
+      <c r="H19" s="25"/>
+      <c r="I19" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
+    <row r="20" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21"/>
       <c r="B20" s="2" t="s">
         <v>62</v>
       </c>
@@ -1869,7 +1870,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="21"/>
+      <c r="H20" s="25"/>
       <c r="I20" s="2" t="s">
         <v>170</v>
       </c>
@@ -1880,19 +1881,19 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="28" t="s">
+      <c r="M20" s="21" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
+    <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="22" t="s">
         <v>116</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1901,8 +1902,8 @@
       <c r="G21" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="27" t="s">
+      <c r="H21" s="25"/>
+      <c r="I21" s="22" t="s">
         <v>169</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1912,25 +1913,25 @@
         <v>178</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="28"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25"/>
+      <c r="M21" s="21"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
       <c r="B22" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="27"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="27"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="22"/>
       <c r="J22" s="1" t="s">
         <v>166</v>
       </c>
@@ -1938,25 +1939,25 @@
         <v>179</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="28"/>
-    </row>
-    <row r="23" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25"/>
+      <c r="M22" s="21"/>
+    </row>
+    <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
       <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="27"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="1" t="s">
         <v>112</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="21"/>
-      <c r="I23" s="27"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="22"/>
       <c r="J23" s="1" t="s">
         <v>167</v>
       </c>
@@ -1964,25 +1965,25 @@
         <v>181</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="28"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
+      <c r="M23" s="21"/>
+    </row>
+    <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="21"/>
       <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="27"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="1" t="s">
         <v>109</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H24" s="21"/>
-      <c r="I24" s="27"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="22"/>
       <c r="J24" s="1" t="s">
         <v>168</v>
       </c>
@@ -1990,18 +1991,21 @@
         <v>180</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="28"/>
-    </row>
-    <row r="25" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="27"/>
+      <c r="M24" s="21"/>
+      <c r="O24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="22"/>
       <c r="F25" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H25" s="21"/>
-      <c r="I25" s="27"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="22"/>
       <c r="J25" s="1" t="s">
         <v>171</v>
       </c>
@@ -2009,9 +2013,9 @@
         <v>182</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="28"/>
-    </row>
-    <row r="26" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="21"/>
+    </row>
+    <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -2028,8 +2032,8 @@
       <c r="G26" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="27"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="22"/>
       <c r="J26" s="1" t="s">
         <v>172</v>
       </c>
@@ -2037,10 +2041,10 @@
         <v>183</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="28"/>
-    </row>
-    <row r="27" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="25" t="s">
+      <c r="M26" s="21"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2058,8 +2062,8 @@
       <c r="G27" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="21"/>
-      <c r="I27" s="27"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="22"/>
       <c r="J27" s="1" t="s">
         <v>173</v>
       </c>
@@ -2067,17 +2071,17 @@
         <v>184</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="28"/>
-    </row>
-    <row r="28" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25"/>
+      <c r="M27" s="21"/>
+    </row>
+    <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21"/>
       <c r="B28" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="20" t="s">
         <v>79</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2086,8 +2090,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="21"/>
-      <c r="I28" s="27"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="22"/>
       <c r="J28" s="1" t="s">
         <v>174</v>
       </c>
@@ -2095,25 +2099,25 @@
         <v>185</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="28"/>
-    </row>
-    <row r="29" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
+      <c r="M28" s="21"/>
+    </row>
+    <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
       <c r="B29" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="24"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="21"/>
-      <c r="I29" s="27"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="22"/>
       <c r="J29" s="1" t="s">
         <v>175</v>
       </c>
@@ -2121,25 +2125,25 @@
         <v>186</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="28"/>
-    </row>
-    <row r="30" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
+      <c r="M29" s="21"/>
+    </row>
+    <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="20"/>
       <c r="F30" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="27"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="22"/>
       <c r="J30" s="1" t="s">
         <v>176</v>
       </c>
@@ -2147,25 +2151,25 @@
         <v>187</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="28"/>
-    </row>
-    <row r="31" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
+      <c r="M30" s="21"/>
+    </row>
+    <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="21"/>
       <c r="B31" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="27"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="22"/>
       <c r="J31" s="1" t="s">
         <v>177</v>
       </c>
@@ -2173,103 +2177,103 @@
         <v>188</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="28"/>
-    </row>
-    <row r="32" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="M31" s="21"/>
+    </row>
+    <row r="32" spans="1:15" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="21"/>
       <c r="B32" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="21"/>
+      <c r="H32" s="25"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="2" t="s">
         <v>94</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="24"/>
+      <c r="E33" s="20"/>
       <c r="F33" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="19" t="s">
+      <c r="H33" s="25"/>
+      <c r="I33" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="24"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="21"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="2" t="s">
         <v>97</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="24"/>
+      <c r="E35" s="20"/>
       <c r="F35" s="8" t="s">
         <v>78</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="H35" s="21"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E36" s="24"/>
+      <c r="E36" s="20"/>
       <c r="F36" s="8" t="s">
         <v>85</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H36" s="21"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -2282,21 +2286,21 @@
       <c r="C37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="24"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H37" s="21"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2305,35 +2309,35 @@
       <c r="C38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="8" t="s">
         <v>88</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="21"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H39" s="21"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="2" t="s">
         <v>125</v>
       </c>
@@ -2349,21 +2353,21 @@
       <c r="G40" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H40" s="21"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="23" t="s">
         <v>157</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2372,111 +2376,111 @@
       <c r="G41" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="21"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="20"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H42" s="21"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E43" s="20"/>
+      <c r="E43" s="23"/>
       <c r="F43" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H43" s="21"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="9" t="s">
         <v>155</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H44" s="21"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E45" s="20"/>
+      <c r="E45" s="23"/>
       <c r="F45" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="21"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="20"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="9" t="s">
         <v>156</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="H46" s="21"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,6 +2517,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
     <mergeCell ref="M20:M31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
@@ -2529,9 +2536,6 @@
     <mergeCell ref="I33:K46"/>
     <mergeCell ref="E41:E46"/>
     <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2567,7 +2571,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>116</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2578,7 +2582,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="1" t="s">
         <v>111</v>
       </c>
@@ -2587,7 +2591,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>112</v>
       </c>
@@ -2596,7 +2600,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1" t="s">
         <v>109</v>
       </c>
@@ -2605,7 +2609,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="1" t="s">
         <v>108</v>
       </c>
@@ -2614,7 +2618,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>191</v>
       </c>
@@ -2623,7 +2627,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="1" t="s">
         <v>194</v>
       </c>
@@ -2632,7 +2636,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1" t="s">
         <v>197</v>
       </c>
@@ -2644,26 +2648,26 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
luxiongbo add project table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -786,10 +786,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1. 领域论文表</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>PAPERLINK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -829,6 +825,11 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 领域论文表   
+2. 是否给实验室信息表增加图片属性</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1043,18 +1044,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1064,11 +1065,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1389,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:E46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1410,20 +1411,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1479,7 +1480,7 @@
         <v>28</v>
       </c>
       <c r="H3" s="25"/>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="20" t="s">
         <v>135</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1506,7 +1507,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="25"/>
-      <c r="I4" s="22"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="4" t="s">
         <v>133</v>
       </c>
@@ -1531,7 +1532,7 @@
         <v>29</v>
       </c>
       <c r="H5" s="25"/>
-      <c r="I5" s="22"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="4" t="s">
         <v>134</v>
       </c>
@@ -1594,7 +1595,7 @@
         <v>98</v>
       </c>
       <c r="H8" s="25"/>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="20" t="s">
         <v>144</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1623,7 +1624,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="25"/>
-      <c r="I9" s="22"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="4" t="s">
         <v>140</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>53</v>
       </c>
       <c r="H10" s="25"/>
-      <c r="I10" s="22"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="4" t="s">
         <v>141</v>
       </c>
@@ -1720,7 +1721,7 @@
         <v>55</v>
       </c>
       <c r="H13" s="25"/>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="20" t="s">
         <v>148</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1747,7 +1748,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="25"/>
-      <c r="I14" s="22"/>
+      <c r="I14" s="20"/>
       <c r="J14" s="4" t="s">
         <v>146</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="25"/>
-      <c r="I15" s="22"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="4" t="s">
         <v>147</v>
       </c>
@@ -1810,11 +1811,11 @@
         <v>57</v>
       </c>
       <c r="H17" s="25"/>
-      <c r="I17" s="26" t="s">
+      <c r="I17" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1846,11 +1847,11 @@
         <v>63</v>
       </c>
       <c r="H19" s="25"/>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
@@ -1882,7 +1883,7 @@
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1893,7 +1894,7 @@
       <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="20" t="s">
         <v>116</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1903,7 +1904,7 @@
         <v>110</v>
       </c>
       <c r="H21" s="25"/>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="20" t="s">
         <v>169</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1923,7 +1924,7 @@
       <c r="C22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="22"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="1" t="s">
         <v>111</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>113</v>
       </c>
       <c r="H22" s="25"/>
-      <c r="I22" s="22"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="1" t="s">
         <v>166</v>
       </c>
@@ -1949,7 +1950,7 @@
       <c r="C23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="22"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="1" t="s">
         <v>112</v>
       </c>
@@ -1957,7 +1958,7 @@
         <v>114</v>
       </c>
       <c r="H23" s="25"/>
-      <c r="I23" s="22"/>
+      <c r="I23" s="20"/>
       <c r="J23" s="1" t="s">
         <v>167</v>
       </c>
@@ -1975,7 +1976,7 @@
       <c r="C24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="1" t="s">
         <v>109</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>115</v>
       </c>
       <c r="H24" s="25"/>
-      <c r="I24" s="22"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="1" t="s">
         <v>168</v>
       </c>
@@ -1993,11 +1994,11 @@
       <c r="L24" s="13"/>
       <c r="M24" s="21"/>
       <c r="O24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="22"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="1" t="s">
         <v>108</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>115</v>
       </c>
       <c r="H25" s="25"/>
-      <c r="I25" s="22"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="1" t="s">
         <v>171</v>
       </c>
@@ -2027,13 +2028,13 @@
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="G26" s="17" t="s">
-        <v>192</v>
-      </c>
       <c r="H26" s="25"/>
-      <c r="I26" s="22"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="1" t="s">
         <v>172</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>59</v>
       </c>
       <c r="H27" s="25"/>
-      <c r="I27" s="22"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="1" t="s">
         <v>173</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="H28" s="25"/>
-      <c r="I28" s="22"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="1" t="s">
         <v>174</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>11</v>
       </c>
       <c r="H29" s="25"/>
-      <c r="I29" s="22"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="1" t="s">
         <v>175</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>80</v>
       </c>
       <c r="H30" s="25"/>
-      <c r="I30" s="22"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="1" t="s">
         <v>176</v>
       </c>
@@ -2169,7 +2170,7 @@
         <v>81</v>
       </c>
       <c r="H31" s="25"/>
-      <c r="I31" s="22"/>
+      <c r="I31" s="20"/>
       <c r="J31" s="1" t="s">
         <v>177</v>
       </c>
@@ -2179,7 +2180,7 @@
       <c r="L31" s="13"/>
       <c r="M31" s="21"/>
     </row>
-    <row r="32" spans="1:15" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="2" t="s">
         <v>93</v>
@@ -2197,7 +2198,7 @@
       <c r="H32" s="25"/>
       <c r="L32" s="13"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21"/>
       <c r="B33" s="2" t="s">
         <v>94</v>
@@ -2213,14 +2214,14 @@
         <v>69</v>
       </c>
       <c r="H33" s="25"/>
-      <c r="I33" s="24" t="s">
-        <v>190</v>
+      <c r="I33" s="27" t="s">
+        <v>200</v>
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="24"/>
       <c r="L33" s="13"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21"/>
       <c r="B34" s="2" t="s">
         <v>96</v>
@@ -2241,7 +2242,7 @@
       <c r="K34" s="24"/>
       <c r="L34" s="13"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21"/>
       <c r="B35" s="2" t="s">
         <v>97</v>
@@ -2262,7 +2263,7 @@
       <c r="K35" s="24"/>
       <c r="L35" s="13"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E36" s="20"/>
       <c r="F36" s="8" t="s">
         <v>85</v>
@@ -2276,7 +2277,7 @@
       <c r="K36" s="24"/>
       <c r="L36" s="13"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>118</v>
       </c>
@@ -2299,7 +2300,7 @@
       <c r="K37" s="24"/>
       <c r="L37" s="13"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>130</v>
       </c>
@@ -2322,7 +2323,7 @@
       <c r="K38" s="24"/>
       <c r="L38" s="13"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="2" t="s">
         <v>120</v>
@@ -2336,7 +2337,7 @@
       <c r="K39" s="24"/>
       <c r="L39" s="13"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21"/>
       <c r="B40" s="2" t="s">
         <v>125</v>
@@ -2359,7 +2360,7 @@
       <c r="K40" s="24"/>
       <c r="L40" s="13"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="21"/>
       <c r="B41" s="2" t="s">
         <v>121</v>
@@ -2367,7 +2368,7 @@
       <c r="C41" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="23" t="s">
+      <c r="E41" s="20" t="s">
         <v>157</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2382,7 +2383,7 @@
       <c r="K41" s="24"/>
       <c r="L41" s="13"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="21"/>
       <c r="B42" s="2" t="s">
         <v>92</v>
@@ -2390,7 +2391,7 @@
       <c r="C42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="23"/>
+      <c r="E42" s="20"/>
       <c r="F42" s="9" t="s">
         <v>152</v>
       </c>
@@ -2403,7 +2404,7 @@
       <c r="K42" s="24"/>
       <c r="L42" s="13"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21"/>
       <c r="B43" s="2" t="s">
         <v>122</v>
@@ -2411,7 +2412,7 @@
       <c r="C43" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E43" s="23"/>
+      <c r="E43" s="20"/>
       <c r="F43" s="9" t="s">
         <v>153</v>
       </c>
@@ -2424,13 +2425,13 @@
       <c r="K43" s="24"/>
       <c r="L43" s="13"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="21"/>
       <c r="B44" s="2" t="s">
         <v>123</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="23"/>
+      <c r="E44" s="20"/>
       <c r="F44" s="9" t="s">
         <v>155</v>
       </c>
@@ -2443,7 +2444,7 @@
       <c r="K44" s="24"/>
       <c r="L44" s="13"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="21"/>
       <c r="B45" s="2" t="s">
         <v>126</v>
@@ -2451,7 +2452,7 @@
       <c r="C45" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E45" s="23"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="9" t="s">
         <v>154</v>
       </c>
@@ -2464,13 +2465,13 @@
       <c r="K45" s="24"/>
       <c r="L45" s="13"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21"/>
       <c r="B46" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="23"/>
+      <c r="E46" s="20"/>
       <c r="F46" s="9" t="s">
         <v>156</v>
       </c>
@@ -2483,7 +2484,7 @@
       <c r="K46" s="24"/>
       <c r="L46" s="13"/>
     </row>
-    <row r="47" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -2517,6 +2518,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I33:K46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="H2:H46"/>
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="I21:I31"/>
@@ -2533,9 +2537,6 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="A18:A24"/>
-    <mergeCell ref="I33:K46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2620,54 +2621,54 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
luxiongbo add research table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -98,10 +98,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>RESEARCH_TBL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>RESEARCH_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -830,6 +826,10 @@
   <si>
     <t>1. 领域论文表   
 2. 是否给实验室信息表增加图片属性</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESEARCH_TBL</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -986,7 +986,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1044,12 +1044,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1059,16 +1068,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1390,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1411,25 +1414,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="A1" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1438,19 +1441,19 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>139</v>
+      <c r="H2" s="22" t="s">
+        <v>138</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>8</v>
@@ -1461,8 +1464,8 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
-        <v>45</v>
+      <c r="A3" s="24" t="s">
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -1470,116 +1473,116 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="20" t="s">
-        <v>135</v>
+        <v>27</v>
+      </c>
+      <c r="H3" s="22"/>
+      <c r="I3" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="20"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="21"/>
       <c r="J4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="21"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="20"/>
+        <v>28</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+    <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="21"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="25"/>
+        <v>29</v>
+      </c>
+      <c r="H6" s="22"/>
       <c r="L6" s="13"/>
     </row>
-    <row r="7" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
+    <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="25"/>
+        <v>30</v>
+      </c>
+      <c r="H7" s="22"/>
       <c r="I7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>143</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>9</v>
@@ -1587,115 +1590,115 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="20" t="s">
-        <v>144</v>
+        <v>97</v>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="21" t="s">
+        <v>143</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="20"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E10" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="20"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="22"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="25"/>
+        <v>53</v>
+      </c>
+      <c r="H12" s="22"/>
       <c r="I12" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>8</v>
@@ -1706,174 +1709,174 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="23"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="20" t="s">
-        <v>148</v>
+        <v>54</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="23"/>
+        <v>42</v>
+      </c>
+      <c r="E14" s="26"/>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="20"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="23"/>
+        <v>43</v>
+      </c>
+      <c r="E15" s="26"/>
       <c r="F15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="20"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="23"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="25"/>
+        <v>55</v>
+      </c>
+      <c r="H16" s="22"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="26"/>
+      <c r="F18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="19" t="s">
+      <c r="C19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="13"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="13"/>
+    </row>
+    <row r="20" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="24"/>
+      <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="25"/>
-      <c r="L18" s="13"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="13"/>
-    </row>
-    <row r="20" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="25"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>8</v>
@@ -1882,606 +1885,606 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="21" t="s">
-        <v>198</v>
+      <c r="M20" s="24" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="L21" s="13"/>
+      <c r="M21" s="24"/>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24"/>
+      <c r="B22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L22" s="13"/>
+      <c r="M22" s="24"/>
+    </row>
+    <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="24"/>
+      <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="C23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H23" s="22"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L23" s="13"/>
+      <c r="M23" s="24"/>
+    </row>
+    <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="24"/>
+      <c r="B24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L24" s="13"/>
+      <c r="M24" s="24"/>
+      <c r="O24" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="21"/>
+      <c r="F25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="L21" s="13"/>
-      <c r="M21" s="21"/>
-    </row>
-    <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
-      <c r="B22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="21"/>
-    </row>
-    <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="K23" s="1" t="s">
+      <c r="H25" s="22"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="L23" s="13"/>
-      <c r="M23" s="21"/>
-    </row>
-    <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="L24" s="13"/>
-      <c r="M24" s="21"/>
-      <c r="O24" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="20"/>
-      <c r="F25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="21"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="G26" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="20"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L26" s="13"/>
+      <c r="M26" s="24"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="22"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K27" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L26" s="13"/>
-      <c r="M26" s="21"/>
-    </row>
-    <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="21"/>
+      <c r="M27" s="24"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>79</v>
+        <v>97</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="25"/>
-      <c r="I28" s="20"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="21"/>
+      <c r="M28" s="24"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="20"/>
+        <v>98</v>
+      </c>
+      <c r="E29" s="21"/>
       <c r="F29" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="21"/>
+      <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" s="22"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="L30" s="13"/>
+      <c r="M30" s="24"/>
+    </row>
+    <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="24"/>
+      <c r="B31" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="22"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L31" s="13"/>
+      <c r="M31" s="24"/>
+    </row>
+    <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="24"/>
+      <c r="B32" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="L30" s="13"/>
-      <c r="M30" s="21"/>
-    </row>
-    <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
-      <c r="B31" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="8" t="s">
+      <c r="E32" s="21"/>
+      <c r="F32" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" s="22"/>
+      <c r="L32" s="13"/>
+    </row>
+    <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="24"/>
+      <c r="B33" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="F33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" s="22"/>
+      <c r="I33" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="13"/>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24"/>
+      <c r="B34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="L31" s="13"/>
-      <c r="M31" s="21"/>
-    </row>
-    <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
-      <c r="B32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G32" s="8" t="s">
+      <c r="H34" s="22"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="13"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="24"/>
+      <c r="B35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H32" s="25"/>
-      <c r="L32" s="13"/>
-    </row>
-    <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
-      <c r="B33" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" s="25"/>
-      <c r="I33" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="13"/>
-    </row>
-    <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
-      <c r="B34" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="8" t="s">
+      <c r="E35" s="21"/>
+      <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H34" s="25"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="13"/>
-    </row>
-    <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="20"/>
+      <c r="E36" s="21"/>
       <c r="F36" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G36" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H36" s="25"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="13"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="21"/>
+      <c r="F38" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" s="22"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="13"/>
+    </row>
+    <row r="39" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="13"/>
-    </row>
-    <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="C39" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H39" s="22"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="13"/>
+    </row>
+    <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="24"/>
+      <c r="B40" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H38" s="25"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
-      <c r="L38" s="13"/>
-    </row>
-    <row r="39" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
-      <c r="L39" s="13"/>
-    </row>
-    <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
-      <c r="B40" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="C40" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
+        <v>58</v>
+      </c>
+      <c r="H40" s="22"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="21"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H41" s="22"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="13"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+      <c r="B42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="21"/>
+      <c r="F42" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="H42" s="22"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="24"/>
+      <c r="B43" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H41" s="25"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="13"/>
-    </row>
-    <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
-      <c r="B42" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="9" t="s">
+      <c r="C43" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
-      <c r="L42" s="13"/>
-    </row>
-    <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="21"/>
-      <c r="B43" s="2" t="s">
+      <c r="H43" s="22"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="13"/>
+    </row>
+    <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="24"/>
+      <c r="B44" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="9" t="s">
+      <c r="C44" s="2"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H44" s="22"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="13"/>
+    </row>
+    <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="24"/>
+      <c r="B45" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="21"/>
+      <c r="F45" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H43" s="25"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
-      <c r="L43" s="13"/>
-    </row>
-    <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
-      <c r="B44" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="9" t="s">
+      <c r="G45" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="13"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="24"/>
+      <c r="B46" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="H44" s="25"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
-      <c r="L44" s="13"/>
-    </row>
-    <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
-      <c r="B45" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45" s="9" t="s">
+      <c r="G46" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H45" s="25"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="13"/>
-    </row>
-    <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21"/>
-      <c r="B46" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="H46" s="25"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2518,12 +2521,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="I33:K46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
     <mergeCell ref="M20:M31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
@@ -2537,6 +2534,12 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="A18:A24"/>
+    <mergeCell ref="I33:K46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2562,7 +2565,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -2572,103 +2575,103 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>116</v>
+      <c r="A2" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
luxiongbo add student table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -824,12 +824,13 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>RESEARCH_TBL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>1. 领域论文表   
-2. 是否给实验室信息表增加图片属性</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>RESEARCH_TBL</t>
+2. 是否给实验室信息表增加图片属性
+3. 学生年份表</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -986,7 +987,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1044,35 +1045,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1393,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1414,20 +1412,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1449,7 +1447,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="25" t="s">
         <v>138</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1464,7 +1462,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="19" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1473,8 +1471,8 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>200</v>
+      <c r="E3" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>18</v>
@@ -1482,7 +1480,7 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="21" t="s">
         <v>134</v>
       </c>
@@ -1495,21 +1493,21 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="21"/>
       <c r="J4" s="4" t="s">
         <v>132</v>
@@ -1520,21 +1518,21 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="21"/>
       <c r="J5" s="4" t="s">
         <v>133</v>
@@ -1545,39 +1543,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="25"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="5" t="s">
         <v>141</v>
       </c>
@@ -1590,14 +1588,14 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="21" t="s">
         <v>143</v>
       </c>
@@ -1610,7 +1608,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="24"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1626,7 +1624,7 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="21"/>
       <c r="J9" s="4" t="s">
         <v>139</v>
@@ -1637,14 +1635,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="21" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1653,7 +1651,7 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="21"/>
       <c r="J10" s="4" t="s">
         <v>140</v>
@@ -1663,40 +1661,40 @@
       </c>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+    <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="26"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="25"/>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
+    <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="26"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="5" t="s">
         <v>144</v>
       </c>
@@ -1709,21 +1707,21 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="26"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="21" t="s">
         <v>147</v>
       </c>
@@ -1736,21 +1734,21 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="22"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="21"/>
       <c r="J14" s="4" t="s">
         <v>145</v>
@@ -1761,21 +1759,21 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="26"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="22"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="21"/>
       <c r="J15" s="4" t="s">
         <v>146</v>
@@ -1785,18 +1783,18 @@
       </c>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:13" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="26"/>
+    <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="21"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="25"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>116</v>
       </c>
@@ -1806,23 +1804,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="26"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23" t="s">
+      <c r="H17" s="25"/>
+      <c r="I17" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+    <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1831,34 +1829,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="26"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="25"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+    <row r="19" spans="1:15" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23" t="s">
+      <c r="H19" s="25"/>
+      <c r="I19" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1874,7 +1872,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="22"/>
+      <c r="H20" s="25"/>
       <c r="I20" s="2" t="s">
         <v>169</v>
       </c>
@@ -1885,12 +1883,12 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="24" t="s">
+      <c r="M20" s="19" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
@@ -1906,7 +1904,7 @@
       <c r="G21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="25"/>
       <c r="I21" s="21" t="s">
         <v>168</v>
       </c>
@@ -1917,10 +1915,10 @@
         <v>177</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="24"/>
+      <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
@@ -1934,7 +1932,7 @@
       <c r="G22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="22"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="21"/>
       <c r="J22" s="1" t="s">
         <v>165</v>
@@ -1943,10 +1941,10 @@
         <v>178</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="24"/>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
@@ -1960,7 +1958,7 @@
       <c r="G23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="22"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="21"/>
       <c r="J23" s="1" t="s">
         <v>166</v>
@@ -1969,10 +1967,10 @@
         <v>180</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="24"/>
+      <c r="M23" s="19"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
@@ -1986,7 +1984,7 @@
       <c r="G24" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="22"/>
+      <c r="H24" s="25"/>
       <c r="I24" s="21"/>
       <c r="J24" s="1" t="s">
         <v>167</v>
@@ -1995,7 +1993,7 @@
         <v>179</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="24"/>
+      <c r="M24" s="19"/>
       <c r="O24" t="s">
         <v>198</v>
       </c>
@@ -2008,7 +2006,7 @@
       <c r="G25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="22"/>
+      <c r="H25" s="25"/>
       <c r="I25" s="21"/>
       <c r="J25" s="1" t="s">
         <v>170</v>
@@ -2017,7 +2015,7 @@
         <v>181</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="24"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2036,7 +2034,7 @@
       <c r="G26" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H26" s="22"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="21"/>
       <c r="J26" s="1" t="s">
         <v>171</v>
@@ -2045,10 +2043,10 @@
         <v>182</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="24"/>
+      <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="19" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2066,7 +2064,7 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="21"/>
       <c r="J27" s="1" t="s">
         <v>172</v>
@@ -2075,10 +2073,10 @@
         <v>183</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="24"/>
+      <c r="M27" s="19"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="24"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
@@ -2094,7 +2092,7 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="25"/>
       <c r="I28" s="21"/>
       <c r="J28" s="1" t="s">
         <v>173</v>
@@ -2103,10 +2101,10 @@
         <v>184</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="24"/>
+      <c r="M28" s="19"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
@@ -2120,7 +2118,7 @@
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="25"/>
       <c r="I29" s="21"/>
       <c r="J29" s="1" t="s">
         <v>174</v>
@@ -2129,10 +2127,10 @@
         <v>185</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="24"/>
+      <c r="M29" s="19"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
@@ -2146,7 +2144,7 @@
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="22"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="21"/>
       <c r="J30" s="1" t="s">
         <v>175</v>
@@ -2155,10 +2153,10 @@
         <v>186</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="24"/>
+      <c r="M30" s="19"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
@@ -2172,7 +2170,7 @@
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="22"/>
+      <c r="H31" s="25"/>
       <c r="I31" s="21"/>
       <c r="J31" s="1" t="s">
         <v>176</v>
@@ -2181,10 +2179,10 @@
         <v>187</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="24"/>
+      <c r="M31" s="19"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="24"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
@@ -2198,11 +2196,11 @@
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="22"/>
+      <c r="H32" s="25"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
@@ -2216,16 +2214,16 @@
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
@@ -2239,14 +2237,14 @@
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
@@ -2260,10 +2258,10 @@
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2274,10 +2272,10 @@
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="22"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2297,14 +2295,14 @@
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="19" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2320,28 +2318,28 @@
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="2" t="s">
         <v>124</v>
       </c>
@@ -2357,14 +2355,14 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="22"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="24"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2380,14 +2378,14 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
@@ -2401,14 +2399,14 @@
       <c r="G42" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="22"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="24"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="2" t="s">
         <v>121</v>
       </c>
@@ -2422,14 +2420,14 @@
       <c r="G43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="24"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="2" t="s">
         <v>122</v>
       </c>
@@ -2441,14 +2439,14 @@
       <c r="G44" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H44" s="22"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="24"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
@@ -2462,14 +2460,14 @@
       <c r="G45" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
@@ -2481,10 +2479,10 @@
       <c r="G46" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2521,6 +2519,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
     <mergeCell ref="M20:M31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
@@ -2537,9 +2538,6 @@
     <mergeCell ref="I33:K46"/>
     <mergeCell ref="E41:E46"/>
     <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2575,7 +2573,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2586,7 +2584,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
@@ -2595,7 +2593,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
@@ -2604,7 +2602,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
@@ -2613,7 +2611,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
@@ -2622,7 +2620,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1" t="s">
         <v>189</v>
       </c>
@@ -2631,7 +2629,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>192</v>
       </c>
@@ -2640,7 +2638,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
luxiongbo add teacher table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -1045,6 +1045,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1052,9 +1058,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -1065,9 +1068,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E18"/>
+      <selection activeCell="A3" sqref="A3:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1412,20 +1412,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1447,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="26" t="s">
         <v>138</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1462,7 +1462,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1471,7 +1471,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>199</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1480,8 +1480,8 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="21" t="s">
+      <c r="H3" s="26"/>
+      <c r="I3" s="20" t="s">
         <v>134</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1493,22 +1493,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="21"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="4" t="s">
         <v>132</v>
       </c>
@@ -1518,22 +1518,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="22"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="4" t="s">
         <v>133</v>
       </c>
@@ -1543,39 +1543,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="25"/>
+      <c r="H6" s="26"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="25"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="5" t="s">
         <v>141</v>
       </c>
@@ -1588,15 +1588,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="21" t="s">
+      <c r="H8" s="26"/>
+      <c r="I8" s="20" t="s">
         <v>143</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1608,7 +1608,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1624,8 +1624,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="21"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="4" t="s">
         <v>139</v>
       </c>
@@ -1635,14 +1635,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1651,8 +1651,8 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="21"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="4" t="s">
         <v>140</v>
       </c>
@@ -1662,39 +1662,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="26"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="25"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="5" t="s">
         <v>144</v>
       </c>
@@ -1707,22 +1707,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="21" t="s">
+      <c r="H13" s="26"/>
+      <c r="I13" s="20" t="s">
         <v>147</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1734,22 +1734,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="21"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="20"/>
       <c r="J14" s="4" t="s">
         <v>145</v>
       </c>
@@ -1759,22 +1759,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="21"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="4" t="s">
         <v>146</v>
       </c>
@@ -1784,14 +1784,14 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="21"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="25"/>
+      <c r="H16" s="26"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1804,23 +1804,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="21"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26" t="s">
+      <c r="H17" s="26"/>
+      <c r="I17" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="21" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1829,34 +1829,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="21"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="25"/>
+      <c r="H18" s="26"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26" t="s">
+      <c r="H19" s="26"/>
+      <c r="I19" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1872,7 +1872,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="25"/>
+      <c r="H20" s="26"/>
       <c r="I20" s="2" t="s">
         <v>169</v>
       </c>
@@ -1883,19 +1883,19 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="19" t="s">
+      <c r="M20" s="21" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="20" t="s">
         <v>115</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1904,8 +1904,8 @@
       <c r="G21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="21" t="s">
+      <c r="H21" s="26"/>
+      <c r="I21" s="20" t="s">
         <v>168</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1915,25 +1915,25 @@
         <v>177</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="19"/>
+      <c r="M21" s="21"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
+      <c r="A22" s="21"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="21"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="1" t="s">
         <v>165</v>
       </c>
@@ -1941,25 +1941,25 @@
         <v>178</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="19"/>
+      <c r="M22" s="21"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="21"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="21"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="20"/>
       <c r="J23" s="1" t="s">
         <v>166</v>
       </c>
@@ -1967,25 +1967,25 @@
         <v>180</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="19"/>
+      <c r="M23" s="21"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="21"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="21"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="1" t="s">
         <v>167</v>
       </c>
@@ -1993,21 +1993,21 @@
         <v>179</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="19"/>
+      <c r="M24" s="21"/>
       <c r="O24" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="21"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="21"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="1" t="s">
         <v>170</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>181</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="19"/>
+      <c r="M25" s="21"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2034,8 +2034,8 @@
       <c r="G26" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="21"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="1" t="s">
         <v>171</v>
       </c>
@@ -2043,10 +2043,10 @@
         <v>182</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="19"/>
+      <c r="M26" s="21"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="21" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2064,8 +2064,8 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="21"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="1" t="s">
         <v>172</v>
       </c>
@@ -2073,17 +2073,17 @@
         <v>183</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="19"/>
+      <c r="M27" s="21"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2092,8 +2092,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="25"/>
-      <c r="I28" s="21"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="1" t="s">
         <v>173</v>
       </c>
@@ -2101,25 +2101,25 @@
         <v>184</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="19"/>
+      <c r="M28" s="21"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="21"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="21"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="1" t="s">
         <v>174</v>
       </c>
@@ -2127,25 +2127,25 @@
         <v>185</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="19"/>
+      <c r="M29" s="21"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="21"/>
+      <c r="E30" s="20"/>
       <c r="F30" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="21"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="1" t="s">
         <v>175</v>
       </c>
@@ -2153,25 +2153,25 @@
         <v>186</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="19"/>
+      <c r="M30" s="21"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="21"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="21"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="20"/>
       <c r="J31" s="1" t="s">
         <v>176</v>
       </c>
@@ -2179,103 +2179,103 @@
         <v>187</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="19"/>
+      <c r="M31" s="21"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="19"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="21"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="25"/>
+      <c r="H32" s="26"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="21"/>
+      <c r="E33" s="20"/>
       <c r="F33" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="25"/>
-      <c r="I33" s="23" t="s">
+      <c r="H33" s="26"/>
+      <c r="I33" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="19"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="21"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="25"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="21"/>
+      <c r="E35" s="20"/>
       <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="21"/>
+      <c r="E36" s="20"/>
       <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="25"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2288,21 +2288,21 @@
       <c r="C37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="21"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="21" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2311,35 +2311,35 @@
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="21"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="25"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="2" t="s">
         <v>124</v>
       </c>
@@ -2355,21 +2355,21 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="20" t="s">
         <v>156</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2378,111 +2378,111 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="25"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="21"/>
+      <c r="E42" s="20"/>
       <c r="F42" s="9" t="s">
         <v>151</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="20"/>
       <c r="F43" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="25"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="21"/>
+      <c r="E44" s="20"/>
       <c r="F44" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H44" s="25"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E45" s="21"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H45" s="25"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="21"/>
+      <c r="E46" s="20"/>
       <c r="F46" s="9" t="s">
         <v>155</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H46" s="25"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2519,6 +2519,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I33:K46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="H2:H46"/>
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="I21:I31"/>
@@ -2535,9 +2538,6 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="A18:A24"/>
-    <mergeCell ref="I33:K46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2573,7 +2573,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
@@ -2593,7 +2593,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
@@ -2602,7 +2602,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
@@ -2611,7 +2611,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
@@ -2620,7 +2620,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>189</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="1" t="s">
         <v>192</v>
       </c>
@@ -2638,7 +2638,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
luxiongbo add project belong table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -1045,12 +1045,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1058,15 +1067,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1412,20 +1412,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1447,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="22" t="s">
         <v>138</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1462,7 +1462,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1471,7 +1471,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="26" t="s">
         <v>199</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1480,8 +1480,8 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="20" t="s">
+      <c r="H3" s="22"/>
+      <c r="I3" s="21" t="s">
         <v>134</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1493,22 +1493,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="20"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="21"/>
       <c r="J4" s="4" t="s">
         <v>132</v>
       </c>
@@ -1518,22 +1518,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="20"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="4" t="s">
         <v>133</v>
       </c>
@@ -1543,39 +1543,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="26"/>
+      <c r="H6" s="22"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="5" t="s">
         <v>141</v>
       </c>
@@ -1588,15 +1588,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="20" t="s">
+      <c r="H8" s="22"/>
+      <c r="I8" s="21" t="s">
         <v>143</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1608,7 +1608,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1624,8 +1624,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="20"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="4" t="s">
         <v>139</v>
       </c>
@@ -1635,14 +1635,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="21" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1651,8 +1651,8 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="20"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="4" t="s">
         <v>140</v>
       </c>
@@ -1662,39 +1662,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="26"/>
+      <c r="H11" s="22"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="26"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="5" t="s">
         <v>144</v>
       </c>
@@ -1707,22 +1707,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="20" t="s">
+      <c r="H13" s="22"/>
+      <c r="I13" s="21" t="s">
         <v>147</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1734,22 +1734,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="20"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="4" t="s">
         <v>145</v>
       </c>
@@ -1759,22 +1759,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="20"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="4" t="s">
         <v>146</v>
       </c>
@@ -1784,14 +1784,14 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="26"/>
+      <c r="H16" s="22"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1804,23 +1804,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="19" t="s">
+      <c r="H17" s="22"/>
+      <c r="I17" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="24" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1829,34 +1829,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="26"/>
+      <c r="H18" s="22"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="22"/>
+      <c r="I19" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1872,7 +1872,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="26"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="2" t="s">
         <v>169</v>
       </c>
@@ -1883,19 +1883,19 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="21" t="s">
+      <c r="M20" s="24" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="21" t="s">
         <v>115</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1904,8 +1904,8 @@
       <c r="G21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="26"/>
-      <c r="I21" s="20" t="s">
+      <c r="H21" s="22"/>
+      <c r="I21" s="21" t="s">
         <v>168</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1915,25 +1915,25 @@
         <v>177</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="21"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="21"/>
       <c r="F22" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="26"/>
-      <c r="I22" s="20"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="1" t="s">
         <v>165</v>
       </c>
@@ -1941,25 +1941,25 @@
         <v>178</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="21"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="20"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="26"/>
-      <c r="I23" s="20"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="1" t="s">
         <v>166</v>
       </c>
@@ -1967,25 +1967,25 @@
         <v>180</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="21"/>
+      <c r="M23" s="24"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="20"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="1" t="s">
         <v>167</v>
       </c>
@@ -1993,21 +1993,21 @@
         <v>179</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="21"/>
+      <c r="M24" s="24"/>
       <c r="O24" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="20"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="20"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="1" t="s">
         <v>170</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>181</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="21"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2034,8 +2034,8 @@
       <c r="G26" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H26" s="26"/>
-      <c r="I26" s="20"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="1" t="s">
         <v>171</v>
       </c>
@@ -2043,10 +2043,10 @@
         <v>182</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="21"/>
+      <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="26" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2064,8 +2064,8 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="20"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="1" t="s">
         <v>172</v>
       </c>
@@ -2073,17 +2073,17 @@
         <v>183</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="21"/>
+      <c r="M27" s="24"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="21" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2092,8 +2092,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="26"/>
-      <c r="I28" s="20"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="1" t="s">
         <v>173</v>
       </c>
@@ -2101,25 +2101,25 @@
         <v>184</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="21"/>
+      <c r="M28" s="24"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="20"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="26"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="1" t="s">
         <v>174</v>
       </c>
@@ -2127,25 +2127,25 @@
         <v>185</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="21"/>
+      <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="21"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="20"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="20"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="1" t="s">
         <v>175</v>
       </c>
@@ -2153,25 +2153,25 @@
         <v>186</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="21"/>
+      <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="21"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="20"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="20"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="1" t="s">
         <v>176</v>
       </c>
@@ -2179,103 +2179,103 @@
         <v>187</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="21"/>
+      <c r="M31" s="24"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="20"/>
+      <c r="E32" s="21"/>
       <c r="F32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="26"/>
+      <c r="H32" s="22"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="21"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="20"/>
+      <c r="E33" s="21"/>
       <c r="F33" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="26"/>
-      <c r="I33" s="24" t="s">
+      <c r="H33" s="22"/>
+      <c r="I33" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="21"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="20"/>
+      <c r="E34" s="21"/>
       <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="26"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="20"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="26"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="20"/>
+      <c r="E36" s="21"/>
       <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="26"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2288,21 +2288,21 @@
       <c r="C37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="20"/>
+      <c r="E37" s="21"/>
       <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="26"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="24" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2311,35 +2311,35 @@
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="21"/>
       <c r="F38" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="26"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="26"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="2" t="s">
         <v>124</v>
       </c>
@@ -2355,21 +2355,21 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="26"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="21"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="21" t="s">
         <v>156</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2378,111 +2378,111 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="26"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="20"/>
+      <c r="E42" s="21"/>
       <c r="F42" s="9" t="s">
         <v>151</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="26"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="21"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="20"/>
+      <c r="E43" s="21"/>
       <c r="F43" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="26"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="21"/>
       <c r="F44" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H44" s="26"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="21"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E45" s="20"/>
+      <c r="E45" s="21"/>
       <c r="F45" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H45" s="26"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="20"/>
+      <c r="E46" s="21"/>
       <c r="F46" s="9" t="s">
         <v>155</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H46" s="26"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2519,12 +2519,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="I33:K46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
     <mergeCell ref="M20:M31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
@@ -2538,6 +2532,12 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="A18:A24"/>
+    <mergeCell ref="I33:K46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2573,7 +2573,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
@@ -2593,7 +2593,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
@@ -2602,7 +2602,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
@@ -2611,7 +2611,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
@@ -2620,7 +2620,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>189</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>192</v>
       </c>
@@ -2638,7 +2638,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="1" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
luxiongbo add research belong table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -1045,29 +1045,29 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A35"/>
+      <selection activeCell="A18" sqref="A18:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1412,20 +1412,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1447,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="25" t="s">
         <v>138</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1462,7 +1462,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1471,7 +1471,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="22" t="s">
         <v>199</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1480,7 +1480,7 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="21" t="s">
         <v>134</v>
       </c>
@@ -1493,21 +1493,21 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="21"/>
       <c r="J4" s="4" t="s">
         <v>132</v>
@@ -1518,21 +1518,21 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="21"/>
       <c r="J5" s="4" t="s">
         <v>133</v>
@@ -1543,39 +1543,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="26"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="25"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="26"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="5" t="s">
         <v>141</v>
       </c>
@@ -1588,14 +1588,14 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="21" t="s">
         <v>143</v>
       </c>
@@ -1608,7 +1608,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1624,7 +1624,7 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="21"/>
       <c r="J9" s="4" t="s">
         <v>139</v>
@@ -1635,7 +1635,7 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1651,7 +1651,7 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="21"/>
       <c r="J10" s="4" t="s">
         <v>140</v>
@@ -1662,7 +1662,7 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
@@ -1676,11 +1676,11 @@
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="25"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="5" t="s">
         <v>144</v>
       </c>
@@ -1707,7 +1707,7 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1721,7 +1721,7 @@
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="21" t="s">
         <v>147</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1748,7 +1748,7 @@
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="22"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="21"/>
       <c r="J14" s="4" t="s">
         <v>145</v>
@@ -1759,7 +1759,7 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
@@ -1773,7 +1773,7 @@
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="22"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="21"/>
       <c r="J15" s="4" t="s">
         <v>146</v>
@@ -1791,7 +1791,7 @@
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="25"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1811,16 +1811,16 @@
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23" t="s">
+      <c r="H17" s="25"/>
+      <c r="I17" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="22" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1836,27 +1836,27 @@
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="25"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="1:15" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+    <row r="19" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23" t="s">
+      <c r="H19" s="25"/>
+      <c r="I19" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
+    <row r="20" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1872,7 +1872,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="22"/>
+      <c r="H20" s="25"/>
       <c r="I20" s="2" t="s">
         <v>169</v>
       </c>
@@ -1883,12 +1883,12 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="24" t="s">
+      <c r="M20" s="19" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="G21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="25"/>
       <c r="I21" s="21" t="s">
         <v>168</v>
       </c>
@@ -1915,10 +1915,10 @@
         <v>177</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="24"/>
+      <c r="M21" s="19"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
@@ -1932,7 +1932,7 @@
       <c r="G22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="22"/>
+      <c r="H22" s="25"/>
       <c r="I22" s="21"/>
       <c r="J22" s="1" t="s">
         <v>165</v>
@@ -1941,10 +1941,10 @@
         <v>178</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="24"/>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
@@ -1958,7 +1958,7 @@
       <c r="G23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="22"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="21"/>
       <c r="J23" s="1" t="s">
         <v>166</v>
@@ -1967,10 +1967,10 @@
         <v>180</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="24"/>
+      <c r="M23" s="19"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="G24" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="22"/>
+      <c r="H24" s="25"/>
       <c r="I24" s="21"/>
       <c r="J24" s="1" t="s">
         <v>167</v>
@@ -1993,7 +1993,7 @@
         <v>179</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="24"/>
+      <c r="M24" s="19"/>
       <c r="O24" t="s">
         <v>198</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="G25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="22"/>
+      <c r="H25" s="25"/>
       <c r="I25" s="21"/>
       <c r="J25" s="1" t="s">
         <v>170</v>
@@ -2015,7 +2015,7 @@
         <v>181</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="24"/>
+      <c r="M25" s="19"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2034,7 +2034,7 @@
       <c r="G26" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H26" s="22"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="21"/>
       <c r="J26" s="1" t="s">
         <v>171</v>
@@ -2043,10 +2043,10 @@
         <v>182</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="24"/>
+      <c r="M26" s="19"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="22" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2064,7 +2064,7 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="22"/>
+      <c r="H27" s="25"/>
       <c r="I27" s="21"/>
       <c r="J27" s="1" t="s">
         <v>172</v>
@@ -2073,10 +2073,10 @@
         <v>183</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="24"/>
+      <c r="M27" s="19"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
@@ -2092,7 +2092,7 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="22"/>
+      <c r="H28" s="25"/>
       <c r="I28" s="21"/>
       <c r="J28" s="1" t="s">
         <v>173</v>
@@ -2101,10 +2101,10 @@
         <v>184</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="24"/>
+      <c r="M28" s="19"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
@@ -2118,7 +2118,7 @@
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="H29" s="25"/>
       <c r="I29" s="21"/>
       <c r="J29" s="1" t="s">
         <v>174</v>
@@ -2127,10 +2127,10 @@
         <v>185</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="24"/>
+      <c r="M29" s="19"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
@@ -2144,7 +2144,7 @@
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="22"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="21"/>
       <c r="J30" s="1" t="s">
         <v>175</v>
@@ -2153,10 +2153,10 @@
         <v>186</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="24"/>
+      <c r="M30" s="19"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
@@ -2170,7 +2170,7 @@
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="22"/>
+      <c r="H31" s="25"/>
       <c r="I31" s="21"/>
       <c r="J31" s="1" t="s">
         <v>176</v>
@@ -2179,10 +2179,10 @@
         <v>187</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="24"/>
+      <c r="M31" s="19"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
@@ -2196,11 +2196,11 @@
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="22"/>
+      <c r="H32" s="25"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
@@ -2214,16 +2214,16 @@
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="19" t="s">
+      <c r="H33" s="25"/>
+      <c r="I33" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
@@ -2237,14 +2237,14 @@
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
@@ -2258,10 +2258,10 @@
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2272,10 +2272,10 @@
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="22"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2295,14 +2295,14 @@
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="19" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2318,28 +2318,28 @@
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="24"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="2" t="s">
         <v>124</v>
       </c>
@@ -2355,14 +2355,14 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="22"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="24"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="2" t="s">
         <v>120</v>
       </c>
@@ -2378,14 +2378,14 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
@@ -2399,14 +2399,14 @@
       <c r="G42" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="22"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="24"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="2" t="s">
         <v>121</v>
       </c>
@@ -2420,14 +2420,14 @@
       <c r="G43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="24"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="2" t="s">
         <v>122</v>
       </c>
@@ -2439,14 +2439,14 @@
       <c r="G44" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H44" s="22"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="24"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
@@ -2460,14 +2460,14 @@
       <c r="G45" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="24"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
@@ -2479,10 +2479,10 @@
       <c r="G46" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2519,6 +2519,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
     <mergeCell ref="M20:M31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
@@ -2535,9 +2538,6 @@
     <mergeCell ref="I33:K46"/>
     <mergeCell ref="E41:E46"/>
     <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2573,7 +2573,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="19" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
@@ -2593,7 +2593,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
@@ -2602,7 +2602,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
@@ -2611,7 +2611,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
@@ -2620,7 +2620,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1" t="s">
         <v>189</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>192</v>
       </c>
@@ -2638,7 +2638,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
luxiongbo add paper belong table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -1045,6 +1045,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1052,9 +1058,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -1065,9 +1068,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1412,20 +1412,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1447,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="26" t="s">
         <v>138</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1462,7 +1462,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1471,7 +1471,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>199</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1480,8 +1480,8 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="21" t="s">
+      <c r="H3" s="26"/>
+      <c r="I3" s="20" t="s">
         <v>134</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1493,22 +1493,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="21"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="20"/>
       <c r="J4" s="4" t="s">
         <v>132</v>
       </c>
@@ -1518,22 +1518,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="22"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="20"/>
       <c r="J5" s="4" t="s">
         <v>133</v>
       </c>
@@ -1543,39 +1543,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="25"/>
+      <c r="H6" s="26"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="25"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="5" t="s">
         <v>141</v>
       </c>
@@ -1588,15 +1588,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="21" t="s">
+      <c r="H8" s="26"/>
+      <c r="I8" s="20" t="s">
         <v>143</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1608,7 +1608,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1624,8 +1624,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="21"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="4" t="s">
         <v>139</v>
       </c>
@@ -1635,14 +1635,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1651,8 +1651,8 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="25"/>
-      <c r="I10" s="21"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="4" t="s">
         <v>140</v>
       </c>
@@ -1662,39 +1662,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="25"/>
+      <c r="H11" s="26"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="25"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="5" t="s">
         <v>144</v>
       </c>
@@ -1707,22 +1707,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="20"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="21" t="s">
+      <c r="H13" s="26"/>
+      <c r="I13" s="20" t="s">
         <v>147</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1734,22 +1734,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="20"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="21"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="20"/>
       <c r="J14" s="4" t="s">
         <v>145</v>
       </c>
@@ -1759,22 +1759,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="21"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="20"/>
       <c r="J15" s="4" t="s">
         <v>146</v>
       </c>
@@ -1784,14 +1784,14 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="21"/>
+      <c r="E16" s="20"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="25"/>
+      <c r="H16" s="26"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1804,23 +1804,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="21"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26" t="s">
+      <c r="H17" s="26"/>
+      <c r="I17" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="23" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1829,34 +1829,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="21"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="25"/>
+      <c r="H18" s="26"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="26" t="s">
+      <c r="H19" s="26"/>
+      <c r="I19" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1872,7 +1872,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="25"/>
+      <c r="H20" s="26"/>
       <c r="I20" s="2" t="s">
         <v>169</v>
       </c>
@@ -1883,19 +1883,19 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="19" t="s">
+      <c r="M20" s="21" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="20" t="s">
         <v>115</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1904,8 +1904,8 @@
       <c r="G21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="21" t="s">
+      <c r="H21" s="26"/>
+      <c r="I21" s="20" t="s">
         <v>168</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1915,25 +1915,25 @@
         <v>177</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="19"/>
+      <c r="M21" s="21"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="20"/>
       <c r="F22" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="21"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="1" t="s">
         <v>165</v>
       </c>
@@ -1941,25 +1941,25 @@
         <v>178</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="19"/>
+      <c r="M22" s="21"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="21"/>
+      <c r="E23" s="20"/>
       <c r="F23" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="21"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="20"/>
       <c r="J23" s="1" t="s">
         <v>166</v>
       </c>
@@ -1967,25 +1967,25 @@
         <v>180</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="19"/>
+      <c r="M23" s="21"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="21"/>
+      <c r="E24" s="20"/>
       <c r="F24" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="21"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="20"/>
       <c r="J24" s="1" t="s">
         <v>167</v>
       </c>
@@ -1993,21 +1993,21 @@
         <v>179</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="19"/>
+      <c r="M24" s="21"/>
       <c r="O24" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="21"/>
+      <c r="E25" s="20"/>
       <c r="F25" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="21"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="1" t="s">
         <v>170</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>181</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="19"/>
+      <c r="M25" s="21"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2034,8 +2034,8 @@
       <c r="G26" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="21"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="1" t="s">
         <v>171</v>
       </c>
@@ -2043,10 +2043,10 @@
         <v>182</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="19"/>
+      <c r="M26" s="21"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="23" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2064,8 +2064,8 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="21"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="1" t="s">
         <v>172</v>
       </c>
@@ -2073,17 +2073,17 @@
         <v>183</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="19"/>
+      <c r="M27" s="21"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2092,8 +2092,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="25"/>
-      <c r="I28" s="21"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="1" t="s">
         <v>173</v>
       </c>
@@ -2101,25 +2101,25 @@
         <v>184</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="19"/>
+      <c r="M28" s="21"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="21"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="21"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="1" t="s">
         <v>174</v>
       </c>
@@ -2127,25 +2127,25 @@
         <v>185</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="19"/>
+      <c r="M29" s="21"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="21"/>
+      <c r="E30" s="20"/>
       <c r="F30" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="21"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="1" t="s">
         <v>175</v>
       </c>
@@ -2153,25 +2153,25 @@
         <v>186</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="19"/>
+      <c r="M30" s="21"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="21"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="21"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="20"/>
       <c r="J31" s="1" t="s">
         <v>176</v>
       </c>
@@ -2179,103 +2179,103 @@
         <v>187</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="19"/>
+      <c r="M31" s="21"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="21"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="25"/>
+      <c r="H32" s="26"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="21"/>
+      <c r="E33" s="20"/>
       <c r="F33" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="25"/>
-      <c r="I33" s="23" t="s">
+      <c r="H33" s="26"/>
+      <c r="I33" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="21"/>
+      <c r="E34" s="20"/>
       <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="25"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="22"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="21"/>
+      <c r="E35" s="20"/>
       <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="21"/>
+      <c r="E36" s="20"/>
       <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="25"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2288,21 +2288,21 @@
       <c r="C37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="21"/>
+      <c r="E37" s="20"/>
       <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="25"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="23" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2311,35 +2311,35 @@
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="21"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="25"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="24"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
       <c r="L38" s="13"/>
     </row>
-    <row r="39" spans="1:12" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
+    <row r="39" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="23"/>
       <c r="B39" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
       <c r="L39" s="13"/>
     </row>
-    <row r="40" spans="1:12" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="19"/>
+    <row r="40" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="23"/>
       <c r="B40" s="2" t="s">
         <v>124</v>
       </c>
@@ -2355,21 +2355,21 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="19"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="20" t="s">
         <v>156</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2378,111 +2378,111 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="25"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="21"/>
+      <c r="E42" s="20"/>
       <c r="F42" s="9" t="s">
         <v>151</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="19"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="20"/>
       <c r="F43" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="25"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="19"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="21"/>
+      <c r="E44" s="20"/>
       <c r="F44" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H44" s="25"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="19"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E45" s="21"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H45" s="25"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="19"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="21"/>
+      <c r="E46" s="20"/>
       <c r="F46" s="9" t="s">
         <v>155</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H46" s="25"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2519,6 +2519,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I33:K46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="H2:H46"/>
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="I21:I31"/>
@@ -2535,9 +2538,6 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="A18:A24"/>
-    <mergeCell ref="I33:K46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2573,7 +2573,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="21"/>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
@@ -2593,7 +2593,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
@@ -2602,7 +2602,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
@@ -2611,7 +2611,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
@@ -2620,7 +2620,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="1" t="s">
         <v>189</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="1" t="s">
         <v>192</v>
       </c>
@@ -2638,7 +2638,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="1" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
luxiongbo add research paper table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="237">
   <si>
     <t>TEACHER_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -831,6 +831,149 @@
     <t>1. 领域论文表   
 2. 是否给实验室信息表增加图片属性
 3. 学生年份表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>领域项目表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>领域论文表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>学生年份表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPAPER_TBL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPRO_TBL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESEARCH_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRO_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPRO_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPROINTRO_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPROINTRO_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简洁</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPER_ID</t>
+  </si>
+  <si>
+    <t>PAPER_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPAPER_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPAPERINTRO_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPAPERINTRO_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>STUYEAR_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEAR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>STU_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>STUYEAR_TBL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>STUYEAR_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>STUYEAR_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>年份</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>外键，标记学生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>还差state表，标记项目的状态</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -987,7 +1130,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1045,12 +1188,21 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1060,17 +1212,17 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1389,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:A46"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1412,20 +1564,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,7 +1599,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="22" t="s">
         <v>138</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1462,7 +1614,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1471,7 +1623,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="26" t="s">
         <v>199</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1480,8 +1632,8 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="20" t="s">
+      <c r="H3" s="22"/>
+      <c r="I3" s="21" t="s">
         <v>134</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1493,22 +1645,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="20"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="21"/>
       <c r="J4" s="4" t="s">
         <v>132</v>
       </c>
@@ -1518,22 +1670,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="26"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="20"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="4" t="s">
         <v>133</v>
       </c>
@@ -1543,39 +1695,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="26"/>
+      <c r="H6" s="22"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="5" t="s">
         <v>141</v>
       </c>
@@ -1588,15 +1740,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="20" t="s">
+      <c r="H8" s="22"/>
+      <c r="I8" s="21" t="s">
         <v>143</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1608,7 +1760,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1624,8 +1776,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="20"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="4" t="s">
         <v>139</v>
       </c>
@@ -1635,14 +1787,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="21" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1651,8 +1803,8 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="20"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="4" t="s">
         <v>140</v>
       </c>
@@ -1662,39 +1814,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="26"/>
+      <c r="H11" s="22"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="26"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="5" t="s">
         <v>144</v>
       </c>
@@ -1707,22 +1859,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="20" t="s">
+      <c r="H13" s="22"/>
+      <c r="I13" s="21" t="s">
         <v>147</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1734,22 +1886,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="20"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="4" t="s">
         <v>145</v>
       </c>
@@ -1759,22 +1911,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="20"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="4" t="s">
         <v>146</v>
       </c>
@@ -1784,14 +1936,14 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="26"/>
+      <c r="H16" s="22"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1804,23 +1956,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="19" t="s">
+      <c r="H17" s="22"/>
+      <c r="I17" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1829,34 +1981,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="26"/>
+      <c r="H18" s="22"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="19" t="s">
+      <c r="H19" s="22"/>
+      <c r="I19" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -1872,7 +2024,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="26"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="2" t="s">
         <v>169</v>
       </c>
@@ -1883,29 +2035,29 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="21" t="s">
+      <c r="M20" s="24" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="21" t="s">
         <v>115</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>106</v>
+        <v>220</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H21" s="26"/>
-      <c r="I21" s="20" t="s">
+      <c r="H21" s="22"/>
+      <c r="I21" s="21" t="s">
         <v>168</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -1915,25 +2067,25 @@
         <v>177</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="21"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="21"/>
       <c r="F22" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="26"/>
-      <c r="I22" s="20"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="1" t="s">
         <v>165</v>
       </c>
@@ -1941,25 +2093,25 @@
         <v>178</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="21"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="20"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="26"/>
-      <c r="I23" s="20"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="1" t="s">
         <v>166</v>
       </c>
@@ -1967,25 +2119,25 @@
         <v>180</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="21"/>
+      <c r="M23" s="24"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="20"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="20"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="1" t="s">
         <v>167</v>
       </c>
@@ -1993,21 +2145,21 @@
         <v>179</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="21"/>
+      <c r="M24" s="24"/>
       <c r="O24" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="20"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="26"/>
-      <c r="I25" s="20"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="1" t="s">
         <v>170</v>
       </c>
@@ -2015,7 +2167,7 @@
         <v>181</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="21"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2034,8 +2186,8 @@
       <c r="G26" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H26" s="26"/>
-      <c r="I26" s="20"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="1" t="s">
         <v>171</v>
       </c>
@@ -2043,10 +2195,10 @@
         <v>182</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="21"/>
+      <c r="M26" s="24"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="26" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2064,8 +2216,8 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="26"/>
-      <c r="I27" s="20"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="1" t="s">
         <v>172</v>
       </c>
@@ -2073,27 +2225,27 @@
         <v>183</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="21"/>
+      <c r="M27" s="24"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="21" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>70</v>
+        <v>209</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="26"/>
-      <c r="I28" s="20"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="1" t="s">
         <v>173</v>
       </c>
@@ -2101,25 +2253,25 @@
         <v>184</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="21"/>
+      <c r="M28" s="24"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="20"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="26"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="1" t="s">
         <v>174</v>
       </c>
@@ -2127,25 +2279,25 @@
         <v>185</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="21"/>
+      <c r="M29" s="24"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="20"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="26"/>
-      <c r="I30" s="20"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="1" t="s">
         <v>175</v>
       </c>
@@ -2153,25 +2305,25 @@
         <v>186</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="21"/>
+      <c r="M30" s="24"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="20"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="26"/>
-      <c r="I31" s="20"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="1" t="s">
         <v>176</v>
       </c>
@@ -2179,103 +2331,103 @@
         <v>187</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="21"/>
+      <c r="M31" s="24"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="20"/>
+      <c r="E32" s="21"/>
       <c r="F32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="26"/>
+      <c r="H32" s="22"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="20"/>
+      <c r="E33" s="21"/>
       <c r="F33" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="26"/>
-      <c r="I33" s="24" t="s">
+      <c r="H33" s="22"/>
+      <c r="I33" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="20"/>
+      <c r="E34" s="21"/>
       <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="26"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
+      <c r="A35" s="26"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="20"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="26"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="20"/>
+      <c r="E36" s="21"/>
       <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="26"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2288,21 +2440,21 @@
       <c r="C37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="20"/>
+      <c r="E37" s="21"/>
       <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="26"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="26" t="s">
         <v>129</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2311,35 +2463,35 @@
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="21"/>
       <c r="F38" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="26"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="26"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="20"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="2" t="s">
         <v>124</v>
       </c>
@@ -2355,21 +2507,21 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="26"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="21" t="s">
         <v>156</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2378,111 +2530,111 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="26"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="20"/>
+      <c r="E42" s="21"/>
       <c r="F42" s="9" t="s">
         <v>151</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="26"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E43" s="20"/>
+      <c r="E43" s="21"/>
       <c r="F43" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="26"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="2" t="s">
         <v>122</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="20"/>
+      <c r="E44" s="21"/>
       <c r="F44" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H44" s="26"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E45" s="20"/>
+      <c r="E45" s="21"/>
       <c r="F45" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H45" s="26"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="20"/>
+      <c r="E46" s="21"/>
       <c r="F46" s="9" t="s">
         <v>155</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="H46" s="26"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2502,29 +2654,196 @@
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>207</v>
+      </c>
       <c r="H49" s="10"/>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>204</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="H50" s="10"/>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="28"/>
+      <c r="B51" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="E51" s="28"/>
+      <c r="F51" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="H51" s="10"/>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="28"/>
+      <c r="J51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="28"/>
+      <c r="B52" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" s="28"/>
+      <c r="F52" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>215</v>
+      </c>
       <c r="H52" s="10"/>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="28"/>
+      <c r="J52" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="28"/>
+      <c r="B53" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="E53" s="28"/>
+      <c r="F53" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="H53" s="11"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="28"/>
+      <c r="B54" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="E54" s="28"/>
+      <c r="F54" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="I54" s="28"/>
+      <c r="J54" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="30"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="I33:K46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
+  <mergeCells count="23">
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="E50:E54"/>
+    <mergeCell ref="I50:I54"/>
+    <mergeCell ref="A56:G58"/>
     <mergeCell ref="M20:M31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
@@ -2538,6 +2857,12 @@
     <mergeCell ref="E10:E18"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="A18:A24"/>
+    <mergeCell ref="I33:K46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2573,7 +2898,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2584,7 +2909,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
@@ -2593,7 +2918,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
@@ -2602,7 +2927,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>108</v>
       </c>
@@ -2611,7 +2936,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
@@ -2620,7 +2945,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="1" t="s">
         <v>189</v>
       </c>
@@ -2629,7 +2954,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="1" t="s">
         <v>192</v>
       </c>
@@ -2638,7 +2963,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="1" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
luxiongbo add research field table
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="总览" sheetId="1" r:id="rId1"/>
-    <sheet name="论文" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="233">
   <si>
     <t>TEACHER_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -450,27 +450,115 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>PAPERBRIEFINTRO_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPERBRIEFINTRO_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPERNAME_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPERNAME_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简介</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPER_TBL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>研究领域从属表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>论文从属表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>字段</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>PAPER_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>PAPERBRIEFINTRO_E</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERBRIEFINTRO_C</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>主键</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERNAME_C</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERNAME_E</t>
+    <t>TACHER_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUTHORTYPE_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUTHORTYPE_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPERBELONG_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPERBELONGISSTU</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPERBELONGINTRO_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPERBELONGINTRO_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否学生</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>作者类型</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAPERBELONG_TBL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDUBKGRD_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDUBKGRD_ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDUBKGRDNAME_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDUBKGRDNAME_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>EDUBKGRD_TBL</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -482,19 +570,23 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>简介</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPER_TBL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>研究领域从属表</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>论文从属表</t>
+    <t>学历表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>左边的表都可以进行读和写，右边的只读，从数据库进行写入</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROFSNTITLENAME_C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROFSNTITLENAME_E</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>职称表</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -502,102 +594,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>PAPER_ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>TACHER_ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUTHORTYPE_C</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUTHORTYPE_E</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERBELONG_ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERBELONGISSTU</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERBELONGINTRO_C</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERBELONGINTRO_E</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否学生</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>作者类型</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERBELONG_TBL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EDUBKGRD_ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EDUBKGRD_ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EDUBKGRDNAME_C</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EDUBKGRDNAME_E</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>EDUBKGRD_TBL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>中文名称</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>英文名称</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>学历表</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>左边的表都可以进行读和写，右边的只读，从数据库进行写入</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PROFSNTITLENAME_C</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PROFSNTITLENAME_E</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>职称表</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>字段</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>PROFSNTITLE_TBL</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -787,32 +783,6 @@
   </si>
   <si>
     <t>论文的链接</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 增加一篇论文或者专利
-2. 修改论文
-3. 删除论文</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERTYPE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>论文类型</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>论文来源</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAPERSOURCE_ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>期刊会议名称</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -974,6 +944,25 @@
   </si>
   <si>
     <t>还差state表，标记项目的状态</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>要新建一个表，应该是大的研究方向的表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>要有中文和英文两个版本</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 左边栏显示研究方向，即领域。
+2. 点击某一研究方向，显示出来领域的详细信息，包括：
+A.  深邃而简洁的图像
+B.  研究方向的标题
+C.  具体的介绍
+D.  相关的论文
+E.  大的标题(研究方向)
+涉及到四个表，研究方向表，研究方向子表，研究方向和研究方向对应表，研究方向子表和论文归属表，其中第一个表可以只传入相关数据即可</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1130,7 +1119,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1188,41 +1177,47 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1543,7 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A56" sqref="A56:G58"/>
     </sheetView>
   </sheetViews>
@@ -1564,20 +1559,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
+      <c r="A1" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1599,11 +1594,11 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>138</v>
+      <c r="H2" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>8</v>
@@ -1614,7 +1609,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1623,8 +1618,8 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>199</v>
+      <c r="E3" s="25" t="s">
+        <v>192</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>18</v>
@@ -1632,12 +1627,12 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="21" t="s">
-        <v>134</v>
+      <c r="H3" s="28"/>
+      <c r="I3" s="24" t="s">
+        <v>133</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>27</v>
@@ -1645,94 +1640,94 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="21"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="24"/>
       <c r="J5" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="26"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="28"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="26"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>9</v>
@@ -1740,16 +1735,16 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="21" t="s">
-        <v>143</v>
+      <c r="H8" s="28"/>
+      <c r="I8" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>2</v>
@@ -1760,7 +1755,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1776,25 +1771,25 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="21"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="24" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1803,52 +1798,52 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="21"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="21"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="28"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="21"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="28"/>
       <c r="I12" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>8</v>
@@ -1859,23 +1854,23 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="24"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="21" t="s">
-        <v>147</v>
+      <c r="H13" s="28"/>
+      <c r="I13" s="24" t="s">
+        <v>146</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>4</v>
@@ -1886,69 +1881,69 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="21"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="21"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="21"/>
+      <c r="E16" s="24"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="22"/>
+      <c r="H16" s="28"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1956,23 +1951,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="21"/>
+      <c r="E17" s="24"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="25" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1981,34 +1976,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="21"/>
+      <c r="E18" s="24"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="22"/>
+      <c r="H18" s="28"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="22"/>
-      <c r="I19" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -2024,9 +2019,9 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="22"/>
+      <c r="H20" s="28"/>
       <c r="I20" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>8</v>
@@ -2035,139 +2030,139 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="24" t="s">
-        <v>197</v>
+      <c r="M20" s="22" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>115</v>
+      <c r="E21" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="21" t="s">
-        <v>168</v>
+        <v>108</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="24" t="s">
+        <v>167</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="24"/>
+      <c r="M21" s="22"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="24"/>
       <c r="F22" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="21"/>
+        <v>111</v>
+      </c>
+      <c r="H22" s="28"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="24"/>
+      <c r="M22" s="22"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="21"/>
+      <c r="E23" s="24"/>
       <c r="F23" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="21"/>
+        <v>112</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="24"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="21"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="21"/>
+        <v>113</v>
+      </c>
+      <c r="H24" s="28"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="24"/>
+      <c r="M24" s="22"/>
       <c r="O24" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="21"/>
+      <c r="E25" s="24"/>
       <c r="F25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="21"/>
+        <v>113</v>
+      </c>
+      <c r="H25" s="28"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="24"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2181,24 +2176,24 @@
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="G26" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="21"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="24"/>
+      <c r="M26" s="22"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="25" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2208,7 +2203,7 @@
         <v>52</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>25</v>
@@ -2216,290 +2211,290 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="21"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="24"/>
+      <c r="M27" s="22"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="24" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="21"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="24"/>
+      <c r="M28" s="22"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="21"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="21"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="24"/>
       <c r="J29" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="24"/>
+      <c r="M29" s="22"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="21"/>
+      <c r="E30" s="24"/>
       <c r="F30" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="21"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="24"/>
       <c r="J30" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="24"/>
+      <c r="M30" s="22"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="21"/>
+      <c r="E31" s="24"/>
       <c r="F31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="21"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="24"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="21"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="22"/>
+      <c r="H32" s="28"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="21"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="21"/>
+      <c r="E34" s="24"/>
       <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="21"/>
+      <c r="E35" s="24"/>
       <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="22"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="21"/>
+      <c r="E36" s="24"/>
       <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="22"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="21"/>
+      <c r="E37" s="24"/>
       <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
-        <v>129</v>
+      <c r="A38" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="21"/>
+      <c r="E38" s="24"/>
       <c r="F38" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="22"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>8</v>
@@ -2507,134 +2502,134 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="22"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="26"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="21" t="s">
-        <v>156</v>
+      <c r="E41" s="24" t="s">
+        <v>155</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="21"/>
+      <c r="E42" s="24"/>
       <c r="F42" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" s="28"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="25"/>
+      <c r="B43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="24"/>
+      <c r="F43" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G43" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="22"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="13"/>
-    </row>
-    <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
-      <c r="B43" s="2" t="s">
+      <c r="H43" s="28"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="13"/>
+    </row>
+    <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="25"/>
+      <c r="B44" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E43" s="21"/>
-      <c r="F43" s="9" t="s">
+      <c r="C44" s="2"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="H44" s="28"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="13"/>
+    </row>
+    <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="25"/>
+      <c r="B45" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="24"/>
+      <c r="F45" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="13"/>
-    </row>
-    <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="26"/>
-      <c r="B44" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="9" t="s">
+      <c r="G45" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" s="28"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="13"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="25"/>
+      <c r="B46" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H44" s="22"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="13"/>
-    </row>
-    <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="26"/>
-      <c r="B45" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E45" s="21"/>
-      <c r="F45" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="G45" s="9" t="s">
+      <c r="G46" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="13"/>
-    </row>
-    <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="26"/>
-      <c r="B46" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2656,195 +2651,192 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H49" s="10"/>
       <c r="I49" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H50" s="10"/>
+      <c r="I50" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="20"/>
+      <c r="B51" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="E51" s="20"/>
+      <c r="F51" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="H51" s="10"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="20"/>
+      <c r="B52" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="C52" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="E52" s="20"/>
+      <c r="F52" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="H52" s="10"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
+      <c r="B53" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="E53" s="20"/>
+      <c r="F53" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H53" s="11"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="B50" s="16" t="s">
+      <c r="C54" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C50" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>204</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="H50" s="10"/>
-      <c r="I50" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="28"/>
-      <c r="B51" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="G51" s="1" t="s">
+      <c r="E54" s="20"/>
+      <c r="F54" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H51" s="10"/>
-      <c r="I51" s="28"/>
-      <c r="J51" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
-      <c r="B52" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="E52" s="28"/>
-      <c r="F52" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="H52" s="10"/>
-      <c r="I52" s="28"/>
-      <c r="J52" s="1" t="s">
+      <c r="I54" s="20"/>
+      <c r="J54" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="K52" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
-      <c r="B53" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>217</v>
-      </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="H53" s="11"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="28"/>
-      <c r="B54" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="E54" s="28"/>
-      <c r="F54" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="I54" s="28"/>
-      <c r="J54" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="B56" s="30"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="30"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="E50:E54"/>
-    <mergeCell ref="I50:I54"/>
-    <mergeCell ref="A56:G58"/>
-    <mergeCell ref="M20:M31"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
     <mergeCell ref="A27:A35"/>
@@ -2861,8 +2853,11 @@
     <mergeCell ref="E41:E46"/>
     <mergeCell ref="H2:H46"/>
     <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="E50:E54"/>
+    <mergeCell ref="I50:I54"/>
+    <mergeCell ref="A56:G58"/>
+    <mergeCell ref="M20:M31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2872,134 +2867,272 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="B3:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="26"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="26"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="26"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="26"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="26"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="26"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="26"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="26"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="26"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="26"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="26"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="26"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="26"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="26"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="26"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A10:C13"/>
-    <mergeCell ref="A2:A9"/>
+  <mergeCells count="3">
+    <mergeCell ref="C3:L18"/>
+    <mergeCell ref="B3:B18"/>
+    <mergeCell ref="B20:L22"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
luxiongbo add research field view
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="237">
   <si>
     <t>TEACHER_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -955,7 +955,32 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1. 左边栏显示研究方向，即领域。
+    <r>
+      <t xml:space="preserve">1. 左边栏显示研究方向，即领域。
+涉及到一个表，研究方向表
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>researchfieldService.getAllResearchfields(true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9C5700"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)  //参数代表是否为中文
 2. 点击某一研究方向，显示出来领域的详细信息，包括：
 A.  深邃而简洁的图像
 B.  研究方向的标题
@@ -963,6 +988,23 @@
 D.  相关的论文
 E.  大的标题(研究方向)
 涉及到四个表，研究方向表，研究方向子表，研究方向和研究方向对应表，研究方向子表和论文归属表，其中第一个表可以只传入相关数据即可</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>researchfieldService.getAllResearchfields(true)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口名称</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试结果</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -970,7 +1012,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,8 +1060,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1065,6 +1115,12 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1119,7 +1175,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1180,6 +1236,27 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1189,35 +1266,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1559,20 +1621,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1594,7 +1656,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="26" t="s">
         <v>137</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1609,7 +1671,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1618,7 +1680,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="23" t="s">
         <v>192</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1627,8 +1689,8 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="26"/>
+      <c r="I3" s="21" t="s">
         <v>133</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1640,22 +1702,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="24"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="21"/>
       <c r="J4" s="4" t="s">
         <v>131</v>
       </c>
@@ -1665,22 +1727,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="24"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="4" t="s">
         <v>132</v>
       </c>
@@ -1690,39 +1752,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="28"/>
+      <c r="H6" s="26"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="28"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="5" t="s">
         <v>140</v>
       </c>
@@ -1735,15 +1797,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="24" t="s">
+      <c r="H8" s="26"/>
+      <c r="I8" s="21" t="s">
         <v>142</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1755,7 +1817,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1771,8 +1833,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="24"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="4" t="s">
         <v>138</v>
       </c>
@@ -1782,14 +1844,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="21" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1798,8 +1860,8 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="24"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="4" t="s">
         <v>139</v>
       </c>
@@ -1809,39 +1871,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="28"/>
+      <c r="H11" s="26"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="24"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="28"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="5" t="s">
         <v>143</v>
       </c>
@@ -1854,22 +1916,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="24"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="24" t="s">
+      <c r="H13" s="26"/>
+      <c r="I13" s="21" t="s">
         <v>146</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1881,22 +1943,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="24"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="24"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="4" t="s">
         <v>144</v>
       </c>
@@ -1906,22 +1968,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="24"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="24"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="4" t="s">
         <v>145</v>
       </c>
@@ -1931,14 +1993,14 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="24"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="28"/>
+      <c r="H16" s="26"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1951,23 +2013,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="24"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="29" t="s">
+      <c r="H17" s="26"/>
+      <c r="I17" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="23" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1976,34 +2038,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="28"/>
+      <c r="H18" s="26"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="29" t="s">
+      <c r="H19" s="26"/>
+      <c r="I19" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -2019,7 +2081,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="28"/>
+      <c r="H20" s="26"/>
       <c r="I20" s="2" t="s">
         <v>168</v>
       </c>
@@ -2030,19 +2092,19 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="22" t="s">
+      <c r="M20" s="29" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="21" t="s">
         <v>114</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -2051,8 +2113,8 @@
       <c r="G21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="24" t="s">
+      <c r="H21" s="26"/>
+      <c r="I21" s="21" t="s">
         <v>167</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -2062,25 +2124,25 @@
         <v>176</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="22"/>
+      <c r="M21" s="29"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="24"/>
+      <c r="E22" s="21"/>
       <c r="F22" s="1" t="s">
         <v>109</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="24"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="1" t="s">
         <v>164</v>
       </c>
@@ -2088,25 +2150,25 @@
         <v>177</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="22"/>
+      <c r="M22" s="29"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="24"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="24"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="1" t="s">
         <v>165</v>
       </c>
@@ -2114,25 +2176,25 @@
         <v>179</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="22"/>
+      <c r="M23" s="29"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="24"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="1" t="s">
         <v>166</v>
       </c>
@@ -2140,21 +2202,21 @@
         <v>178</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="22"/>
+      <c r="M24" s="29"/>
       <c r="O24" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="24"/>
+      <c r="E25" s="21"/>
       <c r="F25" s="1" t="s">
         <v>106</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="24"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="1" t="s">
         <v>169</v>
       </c>
@@ -2162,7 +2224,7 @@
         <v>180</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="22"/>
+      <c r="M25" s="29"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2181,8 +2243,8 @@
       <c r="G26" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="24"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="1" t="s">
         <v>170</v>
       </c>
@@ -2190,10 +2252,10 @@
         <v>181</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="22"/>
+      <c r="M26" s="29"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="23" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2211,8 +2273,8 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="24"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="1" t="s">
         <v>171</v>
       </c>
@@ -2220,17 +2282,17 @@
         <v>182</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="22"/>
+      <c r="M27" s="29"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="21" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2239,8 +2301,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="24"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="1" t="s">
         <v>172</v>
       </c>
@@ -2248,25 +2310,25 @@
         <v>183</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="22"/>
+      <c r="M28" s="29"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="24"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="28"/>
-      <c r="I29" s="24"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="1" t="s">
         <v>173</v>
       </c>
@@ -2274,25 +2336,25 @@
         <v>184</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="22"/>
+      <c r="M29" s="29"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="24"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="28"/>
-      <c r="I30" s="24"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="1" t="s">
         <v>174</v>
       </c>
@@ -2300,25 +2362,25 @@
         <v>185</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="22"/>
+      <c r="M30" s="29"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="24"/>
+      <c r="E31" s="21"/>
       <c r="F31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="24"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="1" t="s">
         <v>175</v>
       </c>
@@ -2326,103 +2388,103 @@
         <v>186</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="22"/>
+      <c r="M31" s="29"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="21"/>
       <c r="F32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="28"/>
+      <c r="H32" s="26"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="24"/>
+      <c r="E33" s="21"/>
       <c r="F33" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="28"/>
-      <c r="I33" s="26" t="s">
+      <c r="H33" s="26"/>
+      <c r="I33" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="24"/>
+      <c r="E34" s="21"/>
       <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="28"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="24"/>
+      <c r="E35" s="21"/>
       <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="28"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="24"/>
+      <c r="E36" s="21"/>
       <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="28"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2435,21 +2497,21 @@
       <c r="C37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="24"/>
+      <c r="E37" s="21"/>
       <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="28"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="23" t="s">
         <v>128</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2458,35 +2520,35 @@
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="21"/>
       <c r="F38" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="28"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="28"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="25"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="2" t="s">
         <v>123</v>
       </c>
@@ -2502,21 +2564,21 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="28"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="25"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="21" t="s">
         <v>155</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2525,111 +2587,111 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="28"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="25"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="24"/>
+      <c r="E42" s="21"/>
       <c r="F42" s="9" t="s">
         <v>150</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="H42" s="28"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="25"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="24"/>
+      <c r="E43" s="21"/>
       <c r="F43" s="9" t="s">
         <v>151</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H43" s="28"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="25"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="24"/>
+      <c r="E44" s="21"/>
       <c r="F44" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H44" s="28"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="25"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E45" s="24"/>
+      <c r="E45" s="21"/>
       <c r="F45" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H45" s="28"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="25"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="24"/>
+      <c r="E46" s="21"/>
       <c r="F46" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H46" s="28"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2680,7 +2742,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+      <c r="A50" s="27" t="s">
         <v>198</v>
       </c>
       <c r="B50" s="16" t="s">
@@ -2689,7 +2751,7 @@
       <c r="C50" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E50" s="27" t="s">
         <v>197</v>
       </c>
       <c r="F50" s="9" t="s">
@@ -2699,7 +2761,7 @@
         <v>217</v>
       </c>
       <c r="H50" s="10"/>
-      <c r="I50" s="20" t="s">
+      <c r="I50" s="27" t="s">
         <v>223</v>
       </c>
       <c r="J50" s="1" t="s">
@@ -2710,14 +2772,14 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="16" t="s">
         <v>201</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="E51" s="20"/>
+      <c r="E51" s="27"/>
       <c r="F51" s="19" t="s">
         <v>201</v>
       </c>
@@ -2725,7 +2787,7 @@
         <v>209</v>
       </c>
       <c r="H51" s="10"/>
-      <c r="I51" s="20"/>
+      <c r="I51" s="27"/>
       <c r="J51" s="1" t="s">
         <v>221</v>
       </c>
@@ -2734,14 +2796,14 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="16" t="s">
         <v>203</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="E52" s="20"/>
+      <c r="E52" s="27"/>
       <c r="F52" s="1" t="s">
         <v>212</v>
       </c>
@@ -2749,7 +2811,7 @@
         <v>208</v>
       </c>
       <c r="H52" s="10"/>
-      <c r="I52" s="20"/>
+      <c r="I52" s="27"/>
       <c r="J52" s="1" t="s">
         <v>222</v>
       </c>
@@ -2758,14 +2820,14 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
+      <c r="A53" s="27"/>
       <c r="B53" s="16" t="s">
         <v>205</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="E53" s="20"/>
+      <c r="E53" s="27"/>
       <c r="F53" s="1" t="s">
         <v>215</v>
       </c>
@@ -2773,7 +2835,7 @@
         <v>218</v>
       </c>
       <c r="H53" s="11"/>
-      <c r="I53" s="20"/>
+      <c r="I53" s="27"/>
       <c r="J53" s="1" t="s">
         <v>224</v>
       </c>
@@ -2782,21 +2844,21 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
+      <c r="A54" s="27"/>
       <c r="B54" s="16" t="s">
         <v>206</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="E54" s="20"/>
+      <c r="E54" s="27"/>
       <c r="F54" s="1" t="s">
         <v>216</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I54" s="20"/>
+      <c r="I54" s="27"/>
       <c r="J54" s="1" t="s">
         <v>225</v>
       </c>
@@ -2805,36 +2867,43 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="21"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="28"/>
+      <c r="F58" s="28"/>
+      <c r="G58" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A56:G58"/>
+    <mergeCell ref="M20:M31"/>
+    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="E50:E54"/>
+    <mergeCell ref="I50:I54"/>
     <mergeCell ref="I19:K19"/>
     <mergeCell ref="I21:I31"/>
     <mergeCell ref="A1:L1"/>
@@ -2851,13 +2920,6 @@
     <mergeCell ref="A18:A24"/>
     <mergeCell ref="I33:K46"/>
     <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="E50:E54"/>
-    <mergeCell ref="I50:I54"/>
-    <mergeCell ref="A56:G58"/>
-    <mergeCell ref="M20:M31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2867,274 +2929,384 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L22"/>
+  <dimension ref="B2:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="18" max="18" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="O2" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="26"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="26"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="30" t="s">
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="O3" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="34" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="24"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="34"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="24"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="34"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="24"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="34"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="24"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+      <c r="S7" s="34"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="34"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="34"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="24"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="34"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="34"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="34"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="24"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="34"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="24"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="34"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="24"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="34"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="34"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="34"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="19">
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="O16:R16"/>
+    <mergeCell ref="O17:R17"/>
     <mergeCell ref="C3:L18"/>
     <mergeCell ref="B3:B18"/>
     <mergeCell ref="B20:L22"/>
+    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="O14:R14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
luxiongbo add show papersimplview
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -1239,6 +1239,21 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1254,19 +1269,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
@@ -1274,12 +1280,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1621,20 +1621,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1656,7 +1656,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="28" t="s">
         <v>137</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1671,7 +1671,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1680,7 +1680,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="23" t="s">
         <v>192</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1689,8 +1689,8 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="26" t="s">
+      <c r="H3" s="28"/>
+      <c r="I3" s="22" t="s">
         <v>133</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1702,22 +1702,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="26"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="22"/>
       <c r="J4" s="4" t="s">
         <v>131</v>
       </c>
@@ -1727,22 +1727,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="26"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="22"/>
       <c r="J5" s="4" t="s">
         <v>132</v>
       </c>
@@ -1752,39 +1752,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="28"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="5" t="s">
         <v>140</v>
       </c>
@@ -1797,15 +1797,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="26" t="s">
+      <c r="H8" s="28"/>
+      <c r="I8" s="22" t="s">
         <v>142</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1817,7 +1817,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1833,8 +1833,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="26"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="4" t="s">
         <v>138</v>
       </c>
@@ -1844,14 +1844,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="22" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1860,8 +1860,8 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="26"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="22"/>
       <c r="J10" s="4" t="s">
         <v>139</v>
       </c>
@@ -1871,39 +1871,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="26"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="23"/>
+      <c r="H11" s="28"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="26"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="28"/>
       <c r="I12" s="5" t="s">
         <v>143</v>
       </c>
@@ -1916,22 +1916,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="26"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="26" t="s">
+      <c r="H13" s="28"/>
+      <c r="I13" s="22" t="s">
         <v>146</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1943,22 +1943,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="23"/>
-      <c r="I14" s="26"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="4" t="s">
         <v>144</v>
       </c>
@@ -1968,22 +1968,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="26"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="26"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="22"/>
       <c r="J15" s="4" t="s">
         <v>145</v>
       </c>
@@ -1993,14 +1993,14 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="26"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="23"/>
+      <c r="H16" s="28"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2013,23 +2013,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="26"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="24" t="s">
+      <c r="H17" s="28"/>
+      <c r="I17" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="23" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2038,34 +2038,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="26"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="23"/>
+      <c r="H18" s="28"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="24" t="s">
+      <c r="H19" s="28"/>
+      <c r="I19" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -2081,7 +2081,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="28"/>
       <c r="I20" s="2" t="s">
         <v>168</v>
       </c>
@@ -2092,19 +2092,19 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="22" t="s">
+      <c r="M20" s="27" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="22" t="s">
         <v>114</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -2113,8 +2113,8 @@
       <c r="G21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="26" t="s">
+      <c r="H21" s="28"/>
+      <c r="I21" s="22" t="s">
         <v>167</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -2124,25 +2124,25 @@
         <v>176</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="22"/>
+      <c r="M21" s="27"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="26"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="1" t="s">
         <v>109</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="26"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="22"/>
       <c r="J22" s="1" t="s">
         <v>164</v>
       </c>
@@ -2150,25 +2150,25 @@
         <v>177</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="22"/>
+      <c r="M22" s="27"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="26"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="26"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="22"/>
       <c r="J23" s="1" t="s">
         <v>165</v>
       </c>
@@ -2176,25 +2176,25 @@
         <v>179</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="22"/>
+      <c r="M23" s="27"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="26"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="23"/>
-      <c r="I24" s="26"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="22"/>
       <c r="J24" s="1" t="s">
         <v>166</v>
       </c>
@@ -2202,21 +2202,21 @@
         <v>178</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="22"/>
+      <c r="M24" s="27"/>
       <c r="O24" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="26"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="1" t="s">
         <v>106</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H25" s="23"/>
-      <c r="I25" s="26"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="22"/>
       <c r="J25" s="1" t="s">
         <v>169</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>180</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="22"/>
+      <c r="M25" s="27"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2243,8 +2243,8 @@
       <c r="G26" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="26"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="22"/>
       <c r="J26" s="1" t="s">
         <v>170</v>
       </c>
@@ -2252,10 +2252,10 @@
         <v>181</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="22"/>
+      <c r="M26" s="27"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="23" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2273,8 +2273,8 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="23"/>
-      <c r="I27" s="26"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="22"/>
       <c r="J27" s="1" t="s">
         <v>171</v>
       </c>
@@ -2282,17 +2282,17 @@
         <v>182</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="22"/>
+      <c r="M27" s="27"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="26" t="s">
+      <c r="E28" s="22" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2301,8 +2301,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="26"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="22"/>
       <c r="J28" s="1" t="s">
         <v>172</v>
       </c>
@@ -2310,25 +2310,25 @@
         <v>183</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="22"/>
+      <c r="M28" s="27"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="26"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="26"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="22"/>
       <c r="J29" s="1" t="s">
         <v>173</v>
       </c>
@@ -2336,25 +2336,25 @@
         <v>184</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="22"/>
+      <c r="M29" s="27"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="26"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="23"/>
-      <c r="I30" s="26"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="22"/>
       <c r="J30" s="1" t="s">
         <v>174</v>
       </c>
@@ -2362,25 +2362,25 @@
         <v>185</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="22"/>
+      <c r="M30" s="27"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="26"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="23"/>
-      <c r="I31" s="26"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="22"/>
       <c r="J31" s="1" t="s">
         <v>175</v>
       </c>
@@ -2388,103 +2388,103 @@
         <v>186</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="22"/>
+      <c r="M31" s="27"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="26"/>
+      <c r="E32" s="22"/>
       <c r="F32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="23"/>
+      <c r="H32" s="28"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="26"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="23"/>
-      <c r="I33" s="29" t="s">
+      <c r="H33" s="28"/>
+      <c r="I33" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="26"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="23"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="28"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="26"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="23"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="26"/>
+      <c r="E36" s="22"/>
       <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="23"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2497,21 +2497,21 @@
       <c r="C37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="26"/>
+      <c r="E37" s="22"/>
       <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="23"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="23" t="s">
         <v>128</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2520,35 +2520,35 @@
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="26"/>
+      <c r="E38" s="22"/>
       <c r="F38" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="23"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="23"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="2" t="s">
         <v>123</v>
       </c>
@@ -2564,21 +2564,21 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="23"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="28"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="22" t="s">
         <v>155</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2587,111 +2587,111 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="23"/>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="26"/>
+      <c r="E42" s="22"/>
       <c r="F42" s="9" t="s">
         <v>150</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="H42" s="23"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="26"/>
+      <c r="E43" s="22"/>
       <c r="F43" s="9" t="s">
         <v>151</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H43" s="23"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="30"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="26"/>
+      <c r="E44" s="22"/>
       <c r="F44" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H44" s="23"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="28"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E45" s="26"/>
+      <c r="E45" s="22"/>
       <c r="F45" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H45" s="23"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="30"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="26"/>
+      <c r="E46" s="22"/>
       <c r="F46" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H46" s="23"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2742,7 +2742,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
+      <c r="A50" s="30" t="s">
         <v>198</v>
       </c>
       <c r="B50" s="16" t="s">
@@ -2751,7 +2751,7 @@
       <c r="C50" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="E50" s="25" t="s">
+      <c r="E50" s="30" t="s">
         <v>197</v>
       </c>
       <c r="F50" s="9" t="s">
@@ -2761,7 +2761,7 @@
         <v>217</v>
       </c>
       <c r="H50" s="10"/>
-      <c r="I50" s="25" t="s">
+      <c r="I50" s="30" t="s">
         <v>223</v>
       </c>
       <c r="J50" s="1" t="s">
@@ -2772,14 +2772,14 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
+      <c r="A51" s="30"/>
       <c r="B51" s="16" t="s">
         <v>201</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="E51" s="25"/>
+      <c r="E51" s="30"/>
       <c r="F51" s="19" t="s">
         <v>201</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>209</v>
       </c>
       <c r="H51" s="10"/>
-      <c r="I51" s="25"/>
+      <c r="I51" s="30"/>
       <c r="J51" s="1" t="s">
         <v>221</v>
       </c>
@@ -2796,14 +2796,14 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="16" t="s">
         <v>203</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="E52" s="25"/>
+      <c r="E52" s="30"/>
       <c r="F52" s="1" t="s">
         <v>212</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>208</v>
       </c>
       <c r="H52" s="10"/>
-      <c r="I52" s="25"/>
+      <c r="I52" s="30"/>
       <c r="J52" s="1" t="s">
         <v>222</v>
       </c>
@@ -2820,14 +2820,14 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="16" t="s">
         <v>205</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="E53" s="25"/>
+      <c r="E53" s="30"/>
       <c r="F53" s="1" t="s">
         <v>215</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>218</v>
       </c>
       <c r="H53" s="11"/>
-      <c r="I53" s="25"/>
+      <c r="I53" s="30"/>
       <c r="J53" s="1" t="s">
         <v>224</v>
       </c>
@@ -2844,21 +2844,21 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="25"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="16" t="s">
         <v>206</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="E54" s="25"/>
+      <c r="E54" s="30"/>
       <c r="F54" s="1" t="s">
         <v>216</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I54" s="25"/>
+      <c r="I54" s="30"/>
       <c r="J54" s="1" t="s">
         <v>225</v>
       </c>
@@ -2867,36 +2867,45 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="21" t="s">
+      <c r="A56" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="21"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A56:G58"/>
+    <mergeCell ref="M20:M31"/>
+    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="E50:E54"/>
+    <mergeCell ref="I50:I54"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
     <mergeCell ref="A27:A35"/>
@@ -2911,15 +2920,6 @@
     <mergeCell ref="A18:A24"/>
     <mergeCell ref="I33:K46"/>
     <mergeCell ref="E41:E46"/>
-    <mergeCell ref="A56:G58"/>
-    <mergeCell ref="M20:M31"/>
-    <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="E50:E54"/>
-    <mergeCell ref="I50:I54"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2941,350 +2941,353 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
       <c r="S2" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="24" t="s">
         <v>231</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="O3" s="24" t="s">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="O3" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
       <c r="S3" s="20" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
       <c r="S4" s="20"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="29"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
       <c r="S5" s="20"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="29"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
       <c r="S6" s="20"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="29"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
       <c r="S7" s="20"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
       <c r="S8" s="20"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="29"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
       <c r="S9" s="20"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
       <c r="S10" s="20"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="29"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
       <c r="S11" s="20"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="29"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
       <c r="S12" s="20"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="29"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
       <c r="S13" s="20"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="29"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
       <c r="S14" s="20"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="29"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
       <c r="S15" s="20"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="29"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
       <c r="S16" s="20"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="29"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
       <c r="S17" s="20"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="29"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="33" t="s">
+      <c r="B20" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="C3:L18"/>
+    <mergeCell ref="B3:B18"/>
     <mergeCell ref="B20:L22"/>
     <mergeCell ref="O3:R3"/>
     <mergeCell ref="O2:R2"/>
@@ -3301,9 +3304,6 @@
     <mergeCell ref="O14:R14"/>
     <mergeCell ref="O15:R15"/>
     <mergeCell ref="O16:R16"/>
-    <mergeCell ref="O17:R17"/>
-    <mergeCell ref="C3:L18"/>
-    <mergeCell ref="B3:B18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
luxiongbo update test unit
Signed-off-by: jiean001 <421511240@qq.com>
</commit_message>
<xml_diff>
--- a/otherfile/databaseDesign.xlsx
+++ b/otherfile/databaseDesign.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="241">
   <si>
     <t>TEACHER_ID</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1005,6 +1005,22 @@
 E.  大的标题(研究方向)
 涉及到四个表，研究方向表，研究方向子表，研究方向和研究方向对应表，研究方向子表和论文归属表，其中第一个表可以只传入相关数据即可</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>respaperService.getPaperSimpleByResearch(research, true)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取全部研究方向</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取某个子领域下面全部的论文视图</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1069,7 +1085,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1121,6 +1137,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1175,7 +1203,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1239,13 +1267,28 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -1254,20 +1297,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1275,11 +1309,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1621,20 +1664,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1656,7 +1699,7 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="23" t="s">
         <v>137</v>
       </c>
       <c r="I2" s="5" t="s">
@@ -1671,7 +1714,7 @@
       <c r="L2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="28" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1680,7 +1723,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="28" t="s">
         <v>192</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -1689,8 +1732,8 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="22" t="s">
+      <c r="H3" s="23"/>
+      <c r="I3" s="26" t="s">
         <v>133</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1702,22 +1745,22 @@
       <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="4" t="s">
         <v>131</v>
       </c>
@@ -1727,22 +1770,22 @@
       <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="22"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="26"/>
       <c r="J5" s="4" t="s">
         <v>132</v>
       </c>
@@ -1752,39 +1795,39 @@
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="28"/>
+      <c r="H6" s="23"/>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="28"/>
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="28"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="5" t="s">
         <v>140</v>
       </c>
@@ -1797,15 +1840,15 @@
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="2" t="s">
         <v>129</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="22" t="s">
+      <c r="H8" s="23"/>
+      <c r="I8" s="26" t="s">
         <v>142</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1817,7 +1860,7 @@
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1833,8 +1876,8 @@
       <c r="G9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="26"/>
       <c r="J9" s="4" t="s">
         <v>138</v>
       </c>
@@ -1844,14 +1887,14 @@
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="26" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1860,8 +1903,8 @@
       <c r="G10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="26"/>
       <c r="J10" s="4" t="s">
         <v>139</v>
       </c>
@@ -1871,39 +1914,39 @@
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="22"/>
+      <c r="E11" s="26"/>
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="28"/>
+      <c r="H11" s="23"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="22"/>
+      <c r="E12" s="26"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="28"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="5" t="s">
         <v>143</v>
       </c>
@@ -1916,22 +1959,22 @@
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="22"/>
+      <c r="E13" s="26"/>
       <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="22" t="s">
+      <c r="H13" s="23"/>
+      <c r="I13" s="26" t="s">
         <v>146</v>
       </c>
       <c r="J13" s="4" t="s">
@@ -1943,22 +1986,22 @@
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="22"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="26"/>
       <c r="J14" s="4" t="s">
         <v>144</v>
       </c>
@@ -1968,22 +2011,22 @@
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="22"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="28"/>
-      <c r="I15" s="22"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="26"/>
       <c r="J15" s="4" t="s">
         <v>145</v>
       </c>
@@ -1993,14 +2036,14 @@
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E16" s="22"/>
+      <c r="E16" s="26"/>
       <c r="F16" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="28"/>
+      <c r="H16" s="23"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2013,23 +2056,23 @@
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="22"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="29" t="s">
+      <c r="H17" s="23"/>
+      <c r="I17" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="28" t="s">
         <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -2038,34 +2081,34 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="22"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="28"/>
+      <c r="H18" s="23"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="I19" s="29" t="s">
+      <c r="H19" s="23"/>
+      <c r="I19" s="24" t="s">
         <v>162</v>
       </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
@@ -2081,7 +2124,7 @@
       <c r="G20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="28"/>
+      <c r="H20" s="23"/>
       <c r="I20" s="2" t="s">
         <v>168</v>
       </c>
@@ -2092,19 +2135,19 @@
         <v>9</v>
       </c>
       <c r="L20" s="13"/>
-      <c r="M20" s="27" t="s">
+      <c r="M20" s="22" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="26" t="s">
         <v>114</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -2113,8 +2156,8 @@
       <c r="G21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="22" t="s">
+      <c r="H21" s="23"/>
+      <c r="I21" s="26" t="s">
         <v>167</v>
       </c>
       <c r="J21" s="1" t="s">
@@ -2124,25 +2167,25 @@
         <v>176</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="27"/>
+      <c r="M21" s="22"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="22"/>
+      <c r="E22" s="26"/>
       <c r="F22" s="1" t="s">
         <v>109</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="22"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="26"/>
       <c r="J22" s="1" t="s">
         <v>164</v>
       </c>
@@ -2150,25 +2193,25 @@
         <v>177</v>
       </c>
       <c r="L22" s="13"/>
-      <c r="M22" s="27"/>
+      <c r="M22" s="22"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="22"/>
+      <c r="E23" s="26"/>
       <c r="F23" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H23" s="28"/>
-      <c r="I23" s="22"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="26"/>
       <c r="J23" s="1" t="s">
         <v>165</v>
       </c>
@@ -2176,25 +2219,25 @@
         <v>179</v>
       </c>
       <c r="L23" s="13"/>
-      <c r="M23" s="27"/>
+      <c r="M23" s="22"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="22"/>
+      <c r="E24" s="26"/>
       <c r="F24" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H24" s="28"/>
-      <c r="I24" s="22"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="26"/>
       <c r="J24" s="1" t="s">
         <v>166</v>
       </c>
@@ -2202,21 +2245,21 @@
         <v>178</v>
       </c>
       <c r="L24" s="13"/>
-      <c r="M24" s="27"/>
+      <c r="M24" s="22"/>
       <c r="O24" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="22"/>
+      <c r="E25" s="26"/>
       <c r="F25" s="1" t="s">
         <v>106</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="22"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="26"/>
       <c r="J25" s="1" t="s">
         <v>169</v>
       </c>
@@ -2224,7 +2267,7 @@
         <v>180</v>
       </c>
       <c r="L25" s="13"/>
-      <c r="M25" s="27"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -2243,8 +2286,8 @@
       <c r="G26" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="22"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="26"/>
       <c r="J26" s="1" t="s">
         <v>170</v>
       </c>
@@ -2252,10 +2295,10 @@
         <v>181</v>
       </c>
       <c r="L26" s="13"/>
-      <c r="M26" s="27"/>
+      <c r="M26" s="22"/>
     </row>
     <row r="27" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="28" t="s">
         <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2273,8 +2316,8 @@
       <c r="G27" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="28"/>
-      <c r="I27" s="22"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="26"/>
       <c r="J27" s="1" t="s">
         <v>171</v>
       </c>
@@ -2282,17 +2325,17 @@
         <v>182</v>
       </c>
       <c r="L27" s="13"/>
-      <c r="M27" s="27"/>
+      <c r="M27" s="22"/>
     </row>
     <row r="28" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="26" t="s">
         <v>78</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -2301,8 +2344,8 @@
       <c r="G28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="22"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="26"/>
       <c r="J28" s="1" t="s">
         <v>172</v>
       </c>
@@ -2310,25 +2353,25 @@
         <v>183</v>
       </c>
       <c r="L28" s="13"/>
-      <c r="M28" s="27"/>
+      <c r="M28" s="22"/>
     </row>
     <row r="29" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="22"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="8" t="s">
         <v>72</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="28"/>
-      <c r="I29" s="22"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="26"/>
       <c r="J29" s="1" t="s">
         <v>173</v>
       </c>
@@ -2336,25 +2379,25 @@
         <v>184</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="27"/>
+      <c r="M29" s="22"/>
     </row>
     <row r="30" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="22"/>
+      <c r="E30" s="26"/>
       <c r="F30" s="8" t="s">
         <v>71</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="28"/>
-      <c r="I30" s="22"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="26"/>
       <c r="J30" s="1" t="s">
         <v>174</v>
       </c>
@@ -2362,25 +2405,25 @@
         <v>185</v>
       </c>
       <c r="L30" s="13"/>
-      <c r="M30" s="27"/>
+      <c r="M30" s="22"/>
     </row>
     <row r="31" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="22"/>
+      <c r="E31" s="26"/>
       <c r="F31" s="8" t="s">
         <v>75</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="H31" s="28"/>
-      <c r="I31" s="22"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="26"/>
       <c r="J31" s="1" t="s">
         <v>175</v>
       </c>
@@ -2388,103 +2431,103 @@
         <v>186</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="27"/>
+      <c r="M31" s="22"/>
     </row>
     <row r="32" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="22"/>
+      <c r="E32" s="26"/>
       <c r="F32" s="8" t="s">
         <v>73</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="28"/>
+      <c r="H32" s="23"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="22"/>
+      <c r="E33" s="26"/>
       <c r="F33" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="28"/>
-      <c r="I33" s="24" t="s">
+      <c r="H33" s="23"/>
+      <c r="I33" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="22"/>
+      <c r="E34" s="26"/>
       <c r="F34" s="8" t="s">
         <v>76</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H34" s="28"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="22"/>
+      <c r="E35" s="26"/>
       <c r="F35" s="8" t="s">
         <v>77</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="28"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="22"/>
+      <c r="E36" s="26"/>
       <c r="F36" s="8" t="s">
         <v>84</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="28"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2497,21 +2540,21 @@
       <c r="C37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="22"/>
+      <c r="E37" s="26"/>
       <c r="F37" s="8" t="s">
         <v>83</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H37" s="28"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="28" t="s">
         <v>128</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -2520,35 +2563,35 @@
       <c r="C38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="22"/>
+      <c r="E38" s="26"/>
       <c r="F38" s="8" t="s">
         <v>87</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H38" s="28"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
       <c r="L38" s="13"/>
     </row>
     <row r="39" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="2" t="s">
         <v>118</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H39" s="28"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
       <c r="L39" s="13"/>
     </row>
     <row r="40" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="2" t="s">
         <v>123</v>
       </c>
@@ -2564,21 +2607,21 @@
       <c r="G40" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H40" s="28"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
       <c r="L40" s="13"/>
     </row>
     <row r="41" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="2" t="s">
         <v>119</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="26" t="s">
         <v>155</v>
       </c>
       <c r="F41" s="9" t="s">
@@ -2587,111 +2630,111 @@
       <c r="G41" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H41" s="28"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
       <c r="L41" s="13"/>
     </row>
     <row r="42" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="22"/>
+      <c r="E42" s="26"/>
       <c r="F42" s="9" t="s">
         <v>150</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="H42" s="28"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E43" s="22"/>
+      <c r="E43" s="26"/>
       <c r="F43" s="9" t="s">
         <v>151</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="H43" s="28"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="30"/>
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="E44" s="22"/>
+      <c r="E44" s="26"/>
       <c r="F44" s="9" t="s">
         <v>153</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="H44" s="28"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
       <c r="L44" s="13"/>
     </row>
     <row r="45" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="2" t="s">
         <v>124</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E45" s="22"/>
+      <c r="E45" s="26"/>
       <c r="F45" s="9" t="s">
         <v>152</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="H45" s="28"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
       <c r="L45" s="13"/>
     </row>
     <row r="46" spans="1:12" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="E46" s="22"/>
+      <c r="E46" s="26"/>
       <c r="F46" s="9" t="s">
         <v>154</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H46" s="28"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
       <c r="L46" s="13"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -2742,7 +2785,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="25" t="s">
         <v>198</v>
       </c>
       <c r="B50" s="16" t="s">
@@ -2751,7 +2794,7 @@
       <c r="C50" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="E50" s="25" t="s">
         <v>197</v>
       </c>
       <c r="F50" s="9" t="s">
@@ -2761,7 +2804,7 @@
         <v>217</v>
       </c>
       <c r="H50" s="10"/>
-      <c r="I50" s="30" t="s">
+      <c r="I50" s="25" t="s">
         <v>223</v>
       </c>
       <c r="J50" s="1" t="s">
@@ -2772,14 +2815,14 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="16" t="s">
         <v>201</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="E51" s="30"/>
+      <c r="E51" s="25"/>
       <c r="F51" s="19" t="s">
         <v>201</v>
       </c>
@@ -2787,7 +2830,7 @@
         <v>209</v>
       </c>
       <c r="H51" s="10"/>
-      <c r="I51" s="30"/>
+      <c r="I51" s="25"/>
       <c r="J51" s="1" t="s">
         <v>221</v>
       </c>
@@ -2796,14 +2839,14 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="30"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="16" t="s">
         <v>203</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="E52" s="30"/>
+      <c r="E52" s="25"/>
       <c r="F52" s="1" t="s">
         <v>212</v>
       </c>
@@ -2811,7 +2854,7 @@
         <v>208</v>
       </c>
       <c r="H52" s="10"/>
-      <c r="I52" s="30"/>
+      <c r="I52" s="25"/>
       <c r="J52" s="1" t="s">
         <v>222</v>
       </c>
@@ -2820,14 +2863,14 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="16" t="s">
         <v>205</v>
       </c>
       <c r="C53" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="E53" s="30"/>
+      <c r="E53" s="25"/>
       <c r="F53" s="1" t="s">
         <v>215</v>
       </c>
@@ -2835,7 +2878,7 @@
         <v>218</v>
       </c>
       <c r="H53" s="11"/>
-      <c r="I53" s="30"/>
+      <c r="I53" s="25"/>
       <c r="J53" s="1" t="s">
         <v>224</v>
       </c>
@@ -2844,21 +2887,21 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="16" t="s">
         <v>206</v>
       </c>
       <c r="C54" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="E54" s="30"/>
+      <c r="E54" s="25"/>
       <c r="F54" s="1" t="s">
         <v>216</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I54" s="30"/>
+      <c r="I54" s="25"/>
       <c r="J54" s="1" t="s">
         <v>225</v>
       </c>
@@ -2867,45 +2910,36 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A56:G58"/>
-    <mergeCell ref="M20:M31"/>
-    <mergeCell ref="H2:H46"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="E50:E54"/>
-    <mergeCell ref="I50:I54"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:I31"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="E28:E38"/>
     <mergeCell ref="A27:A35"/>
@@ -2920,6 +2954,15 @@
     <mergeCell ref="A18:A24"/>
     <mergeCell ref="I33:K46"/>
     <mergeCell ref="E41:E46"/>
+    <mergeCell ref="A56:G58"/>
+    <mergeCell ref="M20:M31"/>
+    <mergeCell ref="H2:H46"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="E50:E54"/>
+    <mergeCell ref="I50:I54"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:I31"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2932,369 +2975,393 @@
   <dimension ref="B2:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:L18"/>
+      <selection activeCell="O6" sqref="O6:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="18" max="18" width="21.33203125" customWidth="1"/>
+    <col min="14" max="14" width="21.5546875" customWidth="1"/>
+    <col min="18" max="18" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
       <c r="S2" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="31" t="s">
         <v>236</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="O3" s="29" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="N3" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="O3" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="20" t="s">
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="13" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="24"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="20"/>
+    <row r="4" spans="2:19" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="B4" s="29"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="N4" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="O4" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="36" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="24"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
       <c r="S5" s="20"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="24"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
       <c r="S6" s="20"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
       <c r="S7" s="20"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
       <c r="S8" s="20"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="24"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
       <c r="S9" s="20"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="24"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="N10" s="35"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
       <c r="S10" s="20"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="N11" s="35"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
       <c r="S11" s="20"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
       <c r="S12" s="20"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
       <c r="S13" s="20"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
       <c r="S14" s="20"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
       <c r="S15" s="20"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
       <c r="S16" s="20"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="O17" s="29"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="29"/>
-      <c r="R17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="N17" s="35"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
       <c r="S17" s="20"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="33" t="s">
         <v>230</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="31"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="O7:R7"/>
     <mergeCell ref="O17:R17"/>
     <mergeCell ref="C3:L18"/>
     <mergeCell ref="B3:B18"/>
     <mergeCell ref="B20:L22"/>
     <mergeCell ref="O3:R3"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O7:R7"/>
     <mergeCell ref="O8:R8"/>
     <mergeCell ref="O9:R9"/>
     <mergeCell ref="O10:R10"/>

</xml_diff>